<commit_message>
record counter and finalDesign
</commit_message>
<xml_diff>
--- a/src/main/java/output/Normality.xlsx
+++ b/src/main/java/output/Normality.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="33">
   <si>
     <t>Semantics</t>
   </si>
@@ -40,30 +40,30 @@
     <t>Backness</t>
   </si>
   <si>
+    <t>Cl-mid</t>
+  </si>
+  <si>
+    <t>Cent</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>Op-mid</t>
+  </si>
+  <si>
     <t>Mid</t>
   </si>
   <si>
-    <t>Op-mid</t>
+    <t>Back</t>
   </si>
   <si>
     <t>Open</t>
   </si>
   <si>
-    <t>Cl-mid</t>
-  </si>
-  <si>
-    <t>Close</t>
-  </si>
-  <si>
-    <t>Cent</t>
-  </si>
-  <si>
     <t>Front</t>
   </si>
   <si>
-    <t>Back</t>
-  </si>
-  <si>
     <t>MANNER</t>
   </si>
   <si>
@@ -107,6 +107,12 @@
   </si>
   <si>
     <t>Lateral</t>
+  </si>
+  <si>
+    <t>Big</t>
+  </si>
+  <si>
+    <t>Small</t>
   </si>
 </sst>
 </file>
@@ -164,42 +170,67 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="51">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -217,7 +248,9 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
@@ -283,28 +316,28 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="I3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>20</v>
@@ -344,34 +377,69 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" t="n" s="4">
+      <c r="A4" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B4" t="n" s="0">
+        <v>30.0</v>
+      </c>
+      <c r="C4" s="0"/>
+      <c r="D4" t="n" s="8">
         <v>0.4</v>
       </c>
-      <c r="E4" t="n" s="3">
+      <c r="E4" t="n" s="5">
         <v>0.03333333333333333</v>
       </c>
-      <c r="F4" t="n" s="2">
+      <c r="F4" t="n" s="6">
         <v>0.03333333333333333</v>
       </c>
-      <c r="G4" t="n" s="5">
+      <c r="G4" t="n" s="2">
         <v>0.5</v>
       </c>
-      <c r="H4" t="n" s="6">
+      <c r="H4" t="n" s="4">
         <v>0.4</v>
       </c>
-      <c r="I4" t="n" s="8">
+      <c r="I4" t="n" s="9">
         <v>0.7666666666666667</v>
       </c>
-      <c r="J4" t="n" s="7">
+      <c r="J4" t="n" s="3">
         <v>0.06666666666666667</v>
       </c>
-      <c r="K4" t="n" s="9">
+      <c r="K4" t="n" s="7">
         <v>0.43333333333333335</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B5" t="n" s="0">
+        <v>30.0</v>
+      </c>
+      <c r="C5" s="0"/>
+      <c r="D5" t="n" s="32">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E5" t="n" s="29">
+        <v>0.06666666666666667</v>
+      </c>
+      <c r="F5" t="n" s="30">
+        <v>0.0</v>
+      </c>
+      <c r="G5" t="n" s="26">
+        <v>0.36666666666666664</v>
+      </c>
+      <c r="H5" t="n" s="28">
+        <v>0.7333333333333333</v>
+      </c>
+      <c r="I5" t="n" s="33">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="J5" t="n" s="27">
+        <v>0.0</v>
+      </c>
+      <c r="K5" t="n" s="31">
+        <v>0.36666666666666664</v>
       </c>
     </row>
   </sheetData>
@@ -392,7 +460,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -410,7 +478,9 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
@@ -476,28 +546,28 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="I3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>20</v>
@@ -537,34 +607,69 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" t="n" s="12">
+      <c r="A4" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B4" t="n" s="0">
+        <v>30.0</v>
+      </c>
+      <c r="C4" s="0"/>
+      <c r="D4" t="n" s="16">
         <v>0.11333333333333333</v>
       </c>
-      <c r="E4" t="n" s="11">
+      <c r="E4" t="n" s="13">
         <v>0.006666666666666667</v>
       </c>
-      <c r="F4" t="n" s="10">
+      <c r="F4" t="n" s="14">
         <v>0.013333333333333334</v>
       </c>
-      <c r="G4" t="n" s="13">
+      <c r="G4" t="n" s="10">
         <v>0.16</v>
       </c>
-      <c r="H4" t="n" s="14">
+      <c r="H4" t="n" s="12">
         <v>0.13333333333333333</v>
       </c>
-      <c r="I4" t="n" s="16">
+      <c r="I4" t="n" s="17">
         <v>0.26</v>
       </c>
-      <c r="J4" t="n" s="15">
+      <c r="J4" t="n" s="11">
         <v>0.02666666666666667</v>
       </c>
-      <c r="K4" t="n" s="17">
+      <c r="K4" t="n" s="15">
         <v>0.14</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B5" t="n" s="0">
+        <v>30.0</v>
+      </c>
+      <c r="C5" s="0"/>
+      <c r="D5" t="n" s="40">
+        <v>0.0684931506849315</v>
+      </c>
+      <c r="E5" t="n" s="37">
+        <v>0.0136986301369863</v>
+      </c>
+      <c r="F5" t="n" s="38">
+        <v>0.0</v>
+      </c>
+      <c r="G5" t="n" s="34">
+        <v>0.0958904109589041</v>
+      </c>
+      <c r="H5" t="n" s="36">
+        <v>0.19863013698630136</v>
+      </c>
+      <c r="I5" t="n" s="41">
+        <v>0.2876712328767123</v>
+      </c>
+      <c r="J5" t="n" s="35">
+        <v>0.0</v>
+      </c>
+      <c r="K5" t="n" s="39">
+        <v>0.08904109589041095</v>
       </c>
     </row>
   </sheetData>
@@ -585,7 +690,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:W4"/>
+  <dimension ref="A1:W5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -603,7 +708,9 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1"/>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
       <c r="D1" s="1" t="s">
         <v>5</v>
       </c>
@@ -669,28 +776,28 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="I3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>15</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>20</v>
@@ -730,34 +837,69 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" t="n" s="20">
+      <c r="A4" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="B4" t="n" s="0">
+        <v>30.0</v>
+      </c>
+      <c r="C4" s="0"/>
+      <c r="D4" t="n" s="24">
         <v>0.5666666666666667</v>
       </c>
-      <c r="E4" t="n" s="19">
+      <c r="E4" t="n" s="21">
         <v>0.03333333333333333</v>
       </c>
-      <c r="F4" t="n" s="18">
+      <c r="F4" t="n" s="22">
         <v>0.06666666666666667</v>
       </c>
-      <c r="G4" t="n" s="21">
+      <c r="G4" t="n" s="18">
         <v>0.8</v>
       </c>
-      <c r="H4" t="n" s="22">
+      <c r="H4" t="n" s="20">
         <v>0.6666666666666666</v>
       </c>
-      <c r="I4" t="n" s="24">
+      <c r="I4" t="n" s="25">
         <v>1.3</v>
       </c>
-      <c r="J4" t="n" s="23">
+      <c r="J4" t="n" s="19">
         <v>0.13333333333333333</v>
       </c>
-      <c r="K4" t="n" s="25">
+      <c r="K4" t="n" s="23">
         <v>0.7</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="B5" t="n" s="0">
+        <v>30.0</v>
+      </c>
+      <c r="C5" s="0"/>
+      <c r="D5" t="n" s="48">
+        <v>0.3333333333333333</v>
+      </c>
+      <c r="E5" t="n" s="45">
+        <v>0.06666666666666667</v>
+      </c>
+      <c r="F5" t="n" s="46">
+        <v>0.0</v>
+      </c>
+      <c r="G5" t="n" s="42">
+        <v>0.4666666666666667</v>
+      </c>
+      <c r="H5" t="n" s="44">
+        <v>0.9666666666666667</v>
+      </c>
+      <c r="I5" t="n" s="49">
+        <v>1.4</v>
+      </c>
+      <c r="J5" t="n" s="43">
+        <v>0.0</v>
+      </c>
+      <c r="K5" t="n" s="47">
+        <v>0.43333333333333335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Shapiro Wilk first working tests
</commit_message>
<xml_diff>
--- a/src/main/java/output/Normality.xlsx
+++ b/src/main/java/output/Normality.xlsx
@@ -40,28 +40,28 @@
     <t>Backness</t>
   </si>
   <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>Op-mid</t>
+  </si>
+  <si>
     <t>Mid</t>
   </si>
   <si>
+    <t>Front</t>
+  </si>
+  <si>
+    <t>Cent</t>
+  </si>
+  <si>
+    <t>Cl-mid</t>
+  </si>
+  <si>
     <t>Back</t>
   </si>
   <si>
-    <t>Front</t>
-  </si>
-  <si>
     <t>Open</t>
-  </si>
-  <si>
-    <t>Op-mid</t>
-  </si>
-  <si>
-    <t>Close</t>
-  </si>
-  <si>
-    <t>Cent</t>
-  </si>
-  <si>
-    <t>Cl-mid</t>
   </si>
   <si>
     <t>MANNER</t>
@@ -205,293 +205,293 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="true">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="true"/>
   </cellXfs>
@@ -586,28 +586,28 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>20</v>
@@ -654,28 +654,28 @@
         <v>15.0</v>
       </c>
       <c r="C4" s="0"/>
-      <c r="D4" t="n" s="5">
+      <c r="D4" t="n" s="9">
         <v>0.5333333333333333</v>
       </c>
-      <c r="E4" t="n" s="6">
+      <c r="E4" t="n" s="3">
         <v>0.06666666666666667</v>
       </c>
-      <c r="F4" t="n" s="2">
+      <c r="F4" t="n" s="4">
         <v>0.06666666666666667</v>
       </c>
-      <c r="G4" t="n" s="9">
+      <c r="G4" t="n" s="7">
         <v>0.2</v>
       </c>
-      <c r="H4" t="n" s="7">
+      <c r="H4" t="n" s="2">
         <v>0.4666666666666667</v>
       </c>
-      <c r="I4" t="n" s="4">
+      <c r="I4" t="n" s="5">
         <v>0.6</v>
       </c>
-      <c r="J4" t="n" s="8">
+      <c r="J4" t="n" s="6">
         <v>0.2</v>
       </c>
-      <c r="K4" t="n" s="3">
+      <c r="K4" t="n" s="8">
         <v>0.3333333333333333</v>
       </c>
     </row>
@@ -687,28 +687,28 @@
         <v>15.0</v>
       </c>
       <c r="C5" s="0"/>
-      <c r="D5" t="n" s="29">
+      <c r="D5" t="n" s="33">
         <v>0.5333333333333333</v>
       </c>
-      <c r="E5" t="n" s="30">
+      <c r="E5" t="n" s="27">
         <v>0.06666666666666667</v>
       </c>
-      <c r="F5" t="n" s="26">
-        <v>0.0</v>
-      </c>
-      <c r="G5" t="n" s="33">
+      <c r="F5" t="n" s="28">
+        <v>0.0</v>
+      </c>
+      <c r="G5" t="n" s="31">
         <v>0.26666666666666666</v>
       </c>
-      <c r="H5" t="n" s="31">
+      <c r="H5" t="n" s="26">
         <v>0.4</v>
       </c>
-      <c r="I5" t="n" s="28">
+      <c r="I5" t="n" s="29">
         <v>0.8</v>
       </c>
-      <c r="J5" t="n" s="32">
+      <c r="J5" t="n" s="30">
         <v>0.13333333333333333</v>
       </c>
-      <c r="K5" t="n" s="27">
+      <c r="K5" t="n" s="32">
         <v>0.2</v>
       </c>
     </row>
@@ -720,28 +720,28 @@
         <v>15.0</v>
       </c>
       <c r="C6" s="0"/>
-      <c r="D6" t="n" s="53">
+      <c r="D6" t="n" s="57">
         <v>0.4666666666666667</v>
       </c>
-      <c r="E6" t="n" s="54">
+      <c r="E6" t="n" s="51">
         <v>0.13333333333333333</v>
       </c>
-      <c r="F6" t="n" s="50">
-        <v>0.0</v>
-      </c>
-      <c r="G6" t="n" s="57">
+      <c r="F6" t="n" s="52">
+        <v>0.0</v>
+      </c>
+      <c r="G6" t="n" s="55">
         <v>0.3333333333333333</v>
       </c>
-      <c r="H6" t="n" s="55">
+      <c r="H6" t="n" s="50">
         <v>0.5333333333333333</v>
       </c>
-      <c r="I6" t="n" s="52">
+      <c r="I6" t="n" s="53">
         <v>0.6666666666666666</v>
       </c>
-      <c r="J6" t="n" s="56">
-        <v>0.0</v>
-      </c>
-      <c r="K6" t="n" s="51">
+      <c r="J6" t="n" s="54">
+        <v>0.0</v>
+      </c>
+      <c r="K6" t="n" s="56">
         <v>0.4666666666666667</v>
       </c>
     </row>
@@ -753,28 +753,28 @@
         <v>14.0</v>
       </c>
       <c r="C7" s="0"/>
-      <c r="D7" t="n" s="77">
+      <c r="D7" t="n" s="81">
         <v>0.5714285714285714</v>
       </c>
-      <c r="E7" t="n" s="78">
+      <c r="E7" t="n" s="75">
         <v>0.14285714285714285</v>
       </c>
-      <c r="F7" t="n" s="74">
-        <v>0.0</v>
-      </c>
-      <c r="G7" t="n" s="81">
+      <c r="F7" t="n" s="76">
+        <v>0.0</v>
+      </c>
+      <c r="G7" t="n" s="79">
         <v>0.2857142857142857</v>
       </c>
-      <c r="H7" t="n" s="79">
+      <c r="H7" t="n" s="74">
         <v>0.5</v>
       </c>
-      <c r="I7" t="n" s="76">
+      <c r="I7" t="n" s="77">
         <v>0.7857142857142857</v>
       </c>
-      <c r="J7" t="n" s="80">
-        <v>0.0</v>
-      </c>
-      <c r="K7" t="n" s="75">
+      <c r="J7" t="n" s="78">
+        <v>0.0</v>
+      </c>
+      <c r="K7" t="n" s="80">
         <v>0.5</v>
       </c>
     </row>
@@ -786,28 +786,28 @@
         <v>15.0</v>
       </c>
       <c r="C8" s="0"/>
-      <c r="D8" t="n" s="101">
+      <c r="D8" t="n" s="105">
         <v>0.7333333333333333</v>
       </c>
-      <c r="E8" t="n" s="102">
+      <c r="E8" t="n" s="99">
         <v>0.06666666666666667</v>
       </c>
-      <c r="F8" t="n" s="98">
-        <v>0.0</v>
-      </c>
-      <c r="G8" t="n" s="105">
+      <c r="F8" t="n" s="100">
+        <v>0.0</v>
+      </c>
+      <c r="G8" t="n" s="103">
         <v>0.4</v>
       </c>
-      <c r="H8" t="n" s="103">
+      <c r="H8" t="n" s="98">
         <v>0.5333333333333333</v>
       </c>
-      <c r="I8" t="n" s="100">
+      <c r="I8" t="n" s="101">
         <v>0.8666666666666667</v>
       </c>
-      <c r="J8" t="n" s="104">
-        <v>0.0</v>
-      </c>
-      <c r="K8" t="n" s="99">
+      <c r="J8" t="n" s="102">
+        <v>0.0</v>
+      </c>
+      <c r="K8" t="n" s="104">
         <v>0.6666666666666666</v>
       </c>
     </row>
@@ -819,28 +819,28 @@
         <v>15.0</v>
       </c>
       <c r="C9" s="0"/>
-      <c r="D9" t="n" s="125">
+      <c r="D9" t="n" s="129">
         <v>0.4</v>
       </c>
-      <c r="E9" t="n" s="126">
+      <c r="E9" t="n" s="123">
         <v>0.06666666666666667</v>
       </c>
-      <c r="F9" t="n" s="122">
-        <v>0.0</v>
-      </c>
-      <c r="G9" t="n" s="129">
+      <c r="F9" t="n" s="124">
+        <v>0.0</v>
+      </c>
+      <c r="G9" t="n" s="127">
         <v>0.26666666666666666</v>
       </c>
-      <c r="H9" t="n" s="127">
+      <c r="H9" t="n" s="122">
         <v>0.6666666666666666</v>
       </c>
-      <c r="I9" t="n" s="124">
+      <c r="I9" t="n" s="125">
         <v>0.8</v>
       </c>
-      <c r="J9" t="n" s="128">
-        <v>0.0</v>
-      </c>
-      <c r="K9" t="n" s="123">
+      <c r="J9" t="n" s="126">
+        <v>0.0</v>
+      </c>
+      <c r="K9" t="n" s="128">
         <v>0.26666666666666666</v>
       </c>
     </row>
@@ -852,28 +852,28 @@
         <v>15.0</v>
       </c>
       <c r="C10" s="0"/>
-      <c r="D10" t="n" s="149">
+      <c r="D10" t="n" s="153">
         <v>0.6</v>
       </c>
-      <c r="E10" t="n" s="150">
-        <v>0.0</v>
-      </c>
-      <c r="F10" t="n" s="146">
-        <v>0.0</v>
-      </c>
-      <c r="G10" t="n" s="153">
+      <c r="E10" t="n" s="147">
+        <v>0.0</v>
+      </c>
+      <c r="F10" t="n" s="148">
+        <v>0.0</v>
+      </c>
+      <c r="G10" t="n" s="151">
         <v>0.2</v>
       </c>
-      <c r="H10" t="n" s="151">
+      <c r="H10" t="n" s="146">
         <v>0.6666666666666666</v>
       </c>
-      <c r="I10" t="n" s="148">
+      <c r="I10" t="n" s="149">
         <v>1.0</v>
       </c>
-      <c r="J10" t="n" s="152">
-        <v>0.0</v>
-      </c>
-      <c r="K10" t="n" s="147">
+      <c r="J10" t="n" s="150">
+        <v>0.0</v>
+      </c>
+      <c r="K10" t="n" s="152">
         <v>0.4666666666666667</v>
       </c>
     </row>
@@ -885,28 +885,28 @@
         <v>15.0</v>
       </c>
       <c r="C11" s="0"/>
-      <c r="D11" t="n" s="173">
+      <c r="D11" t="n" s="177">
         <v>0.5333333333333333</v>
       </c>
-      <c r="E11" t="n" s="174">
+      <c r="E11" t="n" s="171">
         <v>0.06666666666666667</v>
       </c>
-      <c r="F11" t="n" s="170">
-        <v>0.0</v>
-      </c>
-      <c r="G11" t="n" s="177">
+      <c r="F11" t="n" s="172">
+        <v>0.0</v>
+      </c>
+      <c r="G11" t="n" s="175">
         <v>0.2</v>
       </c>
-      <c r="H11" t="n" s="175">
+      <c r="H11" t="n" s="170">
         <v>0.7333333333333333</v>
       </c>
-      <c r="I11" t="n" s="172">
+      <c r="I11" t="n" s="173">
         <v>0.7333333333333333</v>
       </c>
-      <c r="J11" t="n" s="176">
+      <c r="J11" t="n" s="174">
         <v>0.13333333333333333</v>
       </c>
-      <c r="K11" t="n" s="171">
+      <c r="K11" t="n" s="176">
         <v>0.5333333333333333</v>
       </c>
     </row>
@@ -918,28 +918,28 @@
         <v>15.0</v>
       </c>
       <c r="C12" s="0"/>
-      <c r="D12" t="n" s="197">
+      <c r="D12" t="n" s="201">
         <v>0.4666666666666667</v>
       </c>
-      <c r="E12" t="n" s="198">
+      <c r="E12" t="n" s="195">
         <v>0.13333333333333333</v>
       </c>
-      <c r="F12" t="n" s="194">
-        <v>0.0</v>
-      </c>
-      <c r="G12" t="n" s="201">
+      <c r="F12" t="n" s="196">
+        <v>0.0</v>
+      </c>
+      <c r="G12" t="n" s="199">
         <v>0.2</v>
       </c>
-      <c r="H12" t="n" s="199">
+      <c r="H12" t="n" s="194">
         <v>0.7333333333333333</v>
       </c>
-      <c r="I12" t="n" s="196">
+      <c r="I12" t="n" s="197">
         <v>0.7333333333333333</v>
       </c>
-      <c r="J12" t="n" s="200">
-        <v>0.0</v>
-      </c>
-      <c r="K12" t="n" s="195">
+      <c r="J12" t="n" s="198">
+        <v>0.0</v>
+      </c>
+      <c r="K12" t="n" s="200">
         <v>0.4</v>
       </c>
     </row>
@@ -951,28 +951,28 @@
         <v>15.0</v>
       </c>
       <c r="C13" s="0"/>
-      <c r="D13" t="n" s="221">
+      <c r="D13" t="n" s="225">
         <v>0.26666666666666666</v>
       </c>
-      <c r="E13" t="n" s="222">
+      <c r="E13" t="n" s="219">
         <v>0.2</v>
       </c>
-      <c r="F13" t="n" s="218">
-        <v>0.0</v>
-      </c>
-      <c r="G13" t="n" s="225">
+      <c r="F13" t="n" s="220">
+        <v>0.0</v>
+      </c>
+      <c r="G13" t="n" s="223">
         <v>0.26666666666666666</v>
       </c>
-      <c r="H13" t="n" s="223">
+      <c r="H13" t="n" s="218">
         <v>0.5333333333333333</v>
       </c>
-      <c r="I13" t="n" s="220">
+      <c r="I13" t="n" s="221">
         <v>0.5333333333333333</v>
       </c>
-      <c r="J13" t="n" s="224">
+      <c r="J13" t="n" s="222">
         <v>0.06666666666666667</v>
       </c>
-      <c r="K13" t="n" s="219">
+      <c r="K13" t="n" s="224">
         <v>0.6666666666666666</v>
       </c>
     </row>
@@ -984,28 +984,28 @@
         <v>15.0</v>
       </c>
       <c r="C14" s="0"/>
-      <c r="D14" t="n" s="245">
+      <c r="D14" t="n" s="249">
         <v>0.4</v>
       </c>
-      <c r="E14" t="n" s="246">
-        <v>0.0</v>
-      </c>
-      <c r="F14" t="n" s="242">
-        <v>0.0</v>
-      </c>
-      <c r="G14" t="n" s="249">
+      <c r="E14" t="n" s="243">
+        <v>0.0</v>
+      </c>
+      <c r="F14" t="n" s="244">
+        <v>0.0</v>
+      </c>
+      <c r="G14" t="n" s="247">
         <v>0.4</v>
       </c>
-      <c r="H14" t="n" s="247">
+      <c r="H14" t="n" s="242">
         <v>0.6</v>
       </c>
-      <c r="I14" t="n" s="244">
+      <c r="I14" t="n" s="245">
         <v>0.6666666666666666</v>
       </c>
-      <c r="J14" t="n" s="248">
-        <v>0.0</v>
-      </c>
-      <c r="K14" t="n" s="243">
+      <c r="J14" t="n" s="246">
+        <v>0.0</v>
+      </c>
+      <c r="K14" t="n" s="248">
         <v>0.6666666666666666</v>
       </c>
     </row>
@@ -1017,28 +1017,28 @@
         <v>15.0</v>
       </c>
       <c r="C15" s="0"/>
-      <c r="D15" t="n" s="269">
+      <c r="D15" t="n" s="273">
         <v>0.3333333333333333</v>
       </c>
-      <c r="E15" t="n" s="270">
-        <v>0.0</v>
-      </c>
-      <c r="F15" t="n" s="266">
-        <v>0.0</v>
-      </c>
-      <c r="G15" t="n" s="273">
+      <c r="E15" t="n" s="267">
+        <v>0.0</v>
+      </c>
+      <c r="F15" t="n" s="268">
+        <v>0.0</v>
+      </c>
+      <c r="G15" t="n" s="271">
         <v>0.4</v>
       </c>
-      <c r="H15" t="n" s="271">
+      <c r="H15" t="n" s="266">
         <v>0.4</v>
       </c>
-      <c r="I15" t="n" s="268">
+      <c r="I15" t="n" s="269">
         <v>0.5333333333333333</v>
       </c>
-      <c r="J15" t="n" s="272">
-        <v>0.0</v>
-      </c>
-      <c r="K15" t="n" s="267">
+      <c r="J15" t="n" s="270">
+        <v>0.0</v>
+      </c>
+      <c r="K15" t="n" s="272">
         <v>0.5333333333333333</v>
       </c>
     </row>
@@ -1146,28 +1146,28 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>20</v>
@@ -1214,28 +1214,28 @@
         <v>15.0</v>
       </c>
       <c r="C4" s="0"/>
-      <c r="D4" t="n" s="13">
+      <c r="D4" t="n" s="17">
         <v>0.12658227848101267</v>
       </c>
-      <c r="E4" t="n" s="14">
+      <c r="E4" t="n" s="11">
         <v>0.012658227848101266</v>
       </c>
-      <c r="F4" t="n" s="10">
+      <c r="F4" t="n" s="12">
         <v>0.012658227848101266</v>
       </c>
-      <c r="G4" t="n" s="17">
+      <c r="G4" t="n" s="15">
         <v>0.0379746835443038</v>
       </c>
-      <c r="H4" t="n" s="15">
+      <c r="H4" t="n" s="10">
         <v>0.11392405063291139</v>
       </c>
-      <c r="I4" t="n" s="12">
+      <c r="I4" t="n" s="13">
         <v>0.16455696202531644</v>
       </c>
-      <c r="J4" t="n" s="16">
+      <c r="J4" t="n" s="14">
         <v>0.0379746835443038</v>
       </c>
-      <c r="K4" t="n" s="11">
+      <c r="K4" t="n" s="16">
         <v>0.10126582278481013</v>
       </c>
     </row>
@@ -1247,28 +1247,28 @@
         <v>15.0</v>
       </c>
       <c r="C5" s="0"/>
-      <c r="D5" t="n" s="37">
+      <c r="D5" t="n" s="41">
         <v>0.1375</v>
       </c>
-      <c r="E5" t="n" s="38">
+      <c r="E5" t="n" s="35">
         <v>0.0125</v>
       </c>
-      <c r="F5" t="n" s="34">
-        <v>0.0</v>
-      </c>
-      <c r="G5" t="n" s="41">
+      <c r="F5" t="n" s="36">
+        <v>0.0</v>
+      </c>
+      <c r="G5" t="n" s="39">
         <v>0.075</v>
       </c>
-      <c r="H5" t="n" s="39">
+      <c r="H5" t="n" s="34">
         <v>0.0875</v>
       </c>
-      <c r="I5" t="n" s="36">
+      <c r="I5" t="n" s="37">
         <v>0.25</v>
       </c>
-      <c r="J5" t="n" s="40">
+      <c r="J5" t="n" s="38">
         <v>0.025</v>
       </c>
-      <c r="K5" t="n" s="35">
+      <c r="K5" t="n" s="40">
         <v>0.0375</v>
       </c>
     </row>
@@ -1280,28 +1280,28 @@
         <v>15.0</v>
       </c>
       <c r="C6" s="0"/>
-      <c r="D6" t="n" s="61">
+      <c r="D6" t="n" s="65">
         <v>0.11594202898550725</v>
       </c>
-      <c r="E6" t="n" s="62">
+      <c r="E6" t="n" s="59">
         <v>0.028985507246376812</v>
       </c>
-      <c r="F6" t="n" s="58">
-        <v>0.0</v>
-      </c>
-      <c r="G6" t="n" s="65">
+      <c r="F6" t="n" s="60">
+        <v>0.0</v>
+      </c>
+      <c r="G6" t="n" s="63">
         <v>0.07246376811594203</v>
       </c>
-      <c r="H6" t="n" s="63">
+      <c r="H6" t="n" s="58">
         <v>0.14492753623188406</v>
       </c>
-      <c r="I6" t="n" s="60">
+      <c r="I6" t="n" s="61">
         <v>0.2463768115942029</v>
       </c>
-      <c r="J6" t="n" s="64">
-        <v>0.0</v>
-      </c>
-      <c r="K6" t="n" s="59">
+      <c r="J6" t="n" s="62">
+        <v>0.0</v>
+      </c>
+      <c r="K6" t="n" s="64">
         <v>0.11594202898550725</v>
       </c>
     </row>
@@ -1313,28 +1313,28 @@
         <v>14.0</v>
       </c>
       <c r="C7" s="0"/>
-      <c r="D7" t="n" s="85">
+      <c r="D7" t="n" s="89">
         <v>0.11688311688311688</v>
       </c>
-      <c r="E7" t="n" s="86">
+      <c r="E7" t="n" s="83">
         <v>0.025974025974025976</v>
       </c>
-      <c r="F7" t="n" s="82">
-        <v>0.0</v>
-      </c>
-      <c r="G7" t="n" s="89">
+      <c r="F7" t="n" s="84">
+        <v>0.0</v>
+      </c>
+      <c r="G7" t="n" s="87">
         <v>0.05194805194805195</v>
       </c>
-      <c r="H7" t="n" s="87">
+      <c r="H7" t="n" s="82">
         <v>0.12987012987012986</v>
       </c>
-      <c r="I7" t="n" s="84">
+      <c r="I7" t="n" s="85">
         <v>0.22077922077922077</v>
       </c>
-      <c r="J7" t="n" s="88">
-        <v>0.0</v>
-      </c>
-      <c r="K7" t="n" s="83">
+      <c r="J7" t="n" s="86">
+        <v>0.0</v>
+      </c>
+      <c r="K7" t="n" s="88">
         <v>0.1038961038961039</v>
       </c>
     </row>
@@ -1346,28 +1346,28 @@
         <v>15.0</v>
       </c>
       <c r="C8" s="0"/>
-      <c r="D8" t="n" s="109">
+      <c r="D8" t="n" s="113">
         <v>0.1797752808988764</v>
       </c>
-      <c r="E8" t="n" s="110">
+      <c r="E8" t="n" s="107">
         <v>0.011235955056179775</v>
       </c>
-      <c r="F8" t="n" s="106">
-        <v>0.0</v>
-      </c>
-      <c r="G8" t="n" s="113">
+      <c r="F8" t="n" s="108">
+        <v>0.0</v>
+      </c>
+      <c r="G8" t="n" s="111">
         <v>0.0898876404494382</v>
       </c>
-      <c r="H8" t="n" s="111">
+      <c r="H8" t="n" s="106">
         <v>0.1348314606741573</v>
       </c>
-      <c r="I8" t="n" s="108">
+      <c r="I8" t="n" s="109">
         <v>0.25842696629213485</v>
       </c>
-      <c r="J8" t="n" s="112">
-        <v>0.0</v>
-      </c>
-      <c r="K8" t="n" s="107">
+      <c r="J8" t="n" s="110">
+        <v>0.0</v>
+      </c>
+      <c r="K8" t="n" s="112">
         <v>0.15730337078651685</v>
       </c>
     </row>
@@ -1379,28 +1379,28 @@
         <v>15.0</v>
       </c>
       <c r="C9" s="0"/>
-      <c r="D9" t="n" s="133">
+      <c r="D9" t="n" s="137">
         <v>0.136986301369863</v>
       </c>
-      <c r="E9" t="n" s="134">
+      <c r="E9" t="n" s="131">
         <v>0.0136986301369863</v>
       </c>
-      <c r="F9" t="n" s="130">
-        <v>0.0</v>
-      </c>
-      <c r="G9" t="n" s="137">
+      <c r="F9" t="n" s="132">
+        <v>0.0</v>
+      </c>
+      <c r="G9" t="n" s="135">
         <v>0.0684931506849315</v>
       </c>
-      <c r="H9" t="n" s="135">
+      <c r="H9" t="n" s="130">
         <v>0.1917808219178082</v>
       </c>
-      <c r="I9" t="n" s="132">
+      <c r="I9" t="n" s="133">
         <v>0.3287671232876712</v>
       </c>
-      <c r="J9" t="n" s="136">
-        <v>0.0</v>
-      </c>
-      <c r="K9" t="n" s="131">
+      <c r="J9" t="n" s="134">
+        <v>0.0</v>
+      </c>
+      <c r="K9" t="n" s="136">
         <v>0.0821917808219178</v>
       </c>
     </row>
@@ -1412,28 +1412,28 @@
         <v>15.0</v>
       </c>
       <c r="C10" s="0"/>
-      <c r="D10" t="n" s="157">
+      <c r="D10" t="n" s="161">
         <v>0.1780821917808219</v>
       </c>
-      <c r="E10" t="n" s="158">
-        <v>0.0</v>
-      </c>
-      <c r="F10" t="n" s="154">
-        <v>0.0</v>
-      </c>
-      <c r="G10" t="n" s="161">
+      <c r="E10" t="n" s="155">
+        <v>0.0</v>
+      </c>
+      <c r="F10" t="n" s="156">
+        <v>0.0</v>
+      </c>
+      <c r="G10" t="n" s="159">
         <v>0.0410958904109589</v>
       </c>
-      <c r="H10" t="n" s="159">
+      <c r="H10" t="n" s="154">
         <v>0.1643835616438356</v>
       </c>
-      <c r="I10" t="n" s="156">
+      <c r="I10" t="n" s="157">
         <v>0.2876712328767123</v>
       </c>
-      <c r="J10" t="n" s="160">
-        <v>0.0</v>
-      </c>
-      <c r="K10" t="n" s="155">
+      <c r="J10" t="n" s="158">
+        <v>0.0</v>
+      </c>
+      <c r="K10" t="n" s="160">
         <v>0.0958904109589041</v>
       </c>
     </row>
@@ -1445,28 +1445,28 @@
         <v>15.0</v>
       </c>
       <c r="C11" s="0"/>
-      <c r="D11" t="n" s="181">
+      <c r="D11" t="n" s="185">
         <v>0.10989010989010989</v>
       </c>
-      <c r="E11" t="n" s="182">
+      <c r="E11" t="n" s="179">
         <v>0.01098901098901099</v>
       </c>
-      <c r="F11" t="n" s="178">
-        <v>0.0</v>
-      </c>
-      <c r="G11" t="n" s="185">
+      <c r="F11" t="n" s="180">
+        <v>0.0</v>
+      </c>
+      <c r="G11" t="n" s="183">
         <v>0.06593406593406594</v>
       </c>
-      <c r="H11" t="n" s="183">
+      <c r="H11" t="n" s="178">
         <v>0.18681318681318682</v>
       </c>
-      <c r="I11" t="n" s="180">
+      <c r="I11" t="n" s="181">
         <v>0.21978021978021978</v>
       </c>
-      <c r="J11" t="n" s="184">
+      <c r="J11" t="n" s="182">
         <v>0.02197802197802198</v>
       </c>
-      <c r="K11" t="n" s="179">
+      <c r="K11" t="n" s="184">
         <v>0.13186813186813187</v>
       </c>
     </row>
@@ -1478,28 +1478,28 @@
         <v>15.0</v>
       </c>
       <c r="C12" s="0"/>
-      <c r="D12" t="n" s="205">
+      <c r="D12" t="n" s="209">
         <v>0.1323529411764706</v>
       </c>
-      <c r="E12" t="n" s="206">
+      <c r="E12" t="n" s="203">
         <v>0.029411764705882353</v>
       </c>
-      <c r="F12" t="n" s="202">
-        <v>0.0</v>
-      </c>
-      <c r="G12" t="n" s="209">
+      <c r="F12" t="n" s="204">
+        <v>0.0</v>
+      </c>
+      <c r="G12" t="n" s="207">
         <v>0.04411764705882353</v>
       </c>
-      <c r="H12" t="n" s="207">
+      <c r="H12" t="n" s="202">
         <v>0.19117647058823528</v>
       </c>
-      <c r="I12" t="n" s="204">
+      <c r="I12" t="n" s="205">
         <v>0.27941176470588236</v>
       </c>
-      <c r="J12" t="n" s="208">
-        <v>0.0</v>
-      </c>
-      <c r="K12" t="n" s="203">
+      <c r="J12" t="n" s="206">
+        <v>0.0</v>
+      </c>
+      <c r="K12" t="n" s="208">
         <v>0.11764705882352941</v>
       </c>
     </row>
@@ -1511,28 +1511,28 @@
         <v>15.0</v>
       </c>
       <c r="C13" s="0"/>
-      <c r="D13" t="n" s="229">
+      <c r="D13" t="n" s="233">
         <v>0.08823529411764706</v>
       </c>
-      <c r="E13" t="n" s="230">
+      <c r="E13" t="n" s="227">
         <v>0.04411764705882353</v>
       </c>
-      <c r="F13" t="n" s="226">
-        <v>0.0</v>
-      </c>
-      <c r="G13" t="n" s="233">
+      <c r="F13" t="n" s="228">
+        <v>0.0</v>
+      </c>
+      <c r="G13" t="n" s="231">
         <v>0.07352941176470588</v>
       </c>
-      <c r="H13" t="n" s="231">
+      <c r="H13" t="n" s="226">
         <v>0.20588235294117646</v>
       </c>
-      <c r="I13" t="n" s="228">
+      <c r="I13" t="n" s="229">
         <v>0.22058823529411764</v>
       </c>
-      <c r="J13" t="n" s="232">
+      <c r="J13" t="n" s="230">
         <v>0.014705882352941176</v>
       </c>
-      <c r="K13" t="n" s="227">
+      <c r="K13" t="n" s="232">
         <v>0.17647058823529413</v>
       </c>
     </row>
@@ -1544,28 +1544,28 @@
         <v>15.0</v>
       </c>
       <c r="C14" s="0"/>
-      <c r="D14" t="n" s="253">
+      <c r="D14" t="n" s="257">
         <v>0.12987012987012986</v>
       </c>
-      <c r="E14" t="n" s="254">
-        <v>0.0</v>
-      </c>
-      <c r="F14" t="n" s="250">
-        <v>0.0</v>
-      </c>
-      <c r="G14" t="n" s="257">
+      <c r="E14" t="n" s="251">
+        <v>0.0</v>
+      </c>
+      <c r="F14" t="n" s="252">
+        <v>0.0</v>
+      </c>
+      <c r="G14" t="n" s="255">
         <v>0.09090909090909091</v>
       </c>
-      <c r="H14" t="n" s="255">
+      <c r="H14" t="n" s="250">
         <v>0.15584415584415584</v>
       </c>
-      <c r="I14" t="n" s="252">
+      <c r="I14" t="n" s="253">
         <v>0.22077922077922077</v>
       </c>
-      <c r="J14" t="n" s="256">
-        <v>0.0</v>
-      </c>
-      <c r="K14" t="n" s="251">
+      <c r="J14" t="n" s="254">
+        <v>0.0</v>
+      </c>
+      <c r="K14" t="n" s="256">
         <v>0.15584415584415584</v>
       </c>
     </row>
@@ -1577,28 +1577,28 @@
         <v>15.0</v>
       </c>
       <c r="C15" s="0"/>
-      <c r="D15" t="n" s="277">
+      <c r="D15" t="n" s="281">
         <v>0.1076923076923077</v>
       </c>
-      <c r="E15" t="n" s="278">
-        <v>0.0</v>
-      </c>
-      <c r="F15" t="n" s="274">
-        <v>0.0</v>
-      </c>
-      <c r="G15" t="n" s="281">
+      <c r="E15" t="n" s="275">
+        <v>0.0</v>
+      </c>
+      <c r="F15" t="n" s="276">
+        <v>0.0</v>
+      </c>
+      <c r="G15" t="n" s="279">
         <v>0.1076923076923077</v>
       </c>
-      <c r="H15" t="n" s="279">
+      <c r="H15" t="n" s="274">
         <v>0.16923076923076924</v>
       </c>
-      <c r="I15" t="n" s="276">
+      <c r="I15" t="n" s="277">
         <v>0.24615384615384617</v>
       </c>
-      <c r="J15" t="n" s="280">
-        <v>0.0</v>
-      </c>
-      <c r="K15" t="n" s="275">
+      <c r="J15" t="n" s="278">
+        <v>0.0</v>
+      </c>
+      <c r="K15" t="n" s="280">
         <v>0.13846153846153847</v>
       </c>
     </row>
@@ -1706,28 +1706,28 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>9</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>20</v>
@@ -1774,28 +1774,28 @@
         <v>15.0</v>
       </c>
       <c r="C4" s="0"/>
-      <c r="D4" t="n" s="21">
+      <c r="D4" t="n" s="25">
         <v>0.6666666666666666</v>
       </c>
-      <c r="E4" t="n" s="22">
+      <c r="E4" t="n" s="19">
         <v>0.06666666666666667</v>
       </c>
-      <c r="F4" t="n" s="18">
+      <c r="F4" t="n" s="20">
         <v>0.06666666666666667</v>
       </c>
-      <c r="G4" t="n" s="25">
+      <c r="G4" t="n" s="23">
         <v>0.2</v>
       </c>
-      <c r="H4" t="n" s="23">
+      <c r="H4" t="n" s="18">
         <v>0.6</v>
       </c>
-      <c r="I4" t="n" s="20">
+      <c r="I4" t="n" s="21">
         <v>0.8666666666666667</v>
       </c>
-      <c r="J4" t="n" s="24">
+      <c r="J4" t="n" s="22">
         <v>0.2</v>
       </c>
-      <c r="K4" t="n" s="19">
+      <c r="K4" t="n" s="24">
         <v>0.5333333333333333</v>
       </c>
     </row>
@@ -1807,28 +1807,28 @@
         <v>15.0</v>
       </c>
       <c r="C5" s="0"/>
-      <c r="D5" t="n" s="45">
+      <c r="D5" t="n" s="49">
         <v>0.7333333333333333</v>
       </c>
-      <c r="E5" t="n" s="46">
+      <c r="E5" t="n" s="43">
         <v>0.06666666666666667</v>
       </c>
-      <c r="F5" t="n" s="42">
-        <v>0.0</v>
-      </c>
-      <c r="G5" t="n" s="49">
+      <c r="F5" t="n" s="44">
+        <v>0.0</v>
+      </c>
+      <c r="G5" t="n" s="47">
         <v>0.4</v>
       </c>
-      <c r="H5" t="n" s="47">
+      <c r="H5" t="n" s="42">
         <v>0.4666666666666667</v>
       </c>
-      <c r="I5" t="n" s="44">
+      <c r="I5" t="n" s="45">
         <v>1.3333333333333333</v>
       </c>
-      <c r="J5" t="n" s="48">
+      <c r="J5" t="n" s="46">
         <v>0.13333333333333333</v>
       </c>
-      <c r="K5" t="n" s="43">
+      <c r="K5" t="n" s="48">
         <v>0.2</v>
       </c>
     </row>
@@ -1840,28 +1840,28 @@
         <v>15.0</v>
       </c>
       <c r="C6" s="0"/>
-      <c r="D6" t="n" s="69">
+      <c r="D6" t="n" s="73">
         <v>0.5333333333333333</v>
       </c>
-      <c r="E6" t="n" s="70">
+      <c r="E6" t="n" s="67">
         <v>0.13333333333333333</v>
       </c>
-      <c r="F6" t="n" s="66">
-        <v>0.0</v>
-      </c>
-      <c r="G6" t="n" s="73">
+      <c r="F6" t="n" s="68">
+        <v>0.0</v>
+      </c>
+      <c r="G6" t="n" s="71">
         <v>0.3333333333333333</v>
       </c>
-      <c r="H6" t="n" s="71">
+      <c r="H6" t="n" s="66">
         <v>0.6666666666666666</v>
       </c>
-      <c r="I6" t="n" s="68">
+      <c r="I6" t="n" s="69">
         <v>1.1333333333333333</v>
       </c>
-      <c r="J6" t="n" s="72">
-        <v>0.0</v>
-      </c>
-      <c r="K6" t="n" s="67">
+      <c r="J6" t="n" s="70">
+        <v>0.0</v>
+      </c>
+      <c r="K6" t="n" s="72">
         <v>0.5333333333333333</v>
       </c>
     </row>
@@ -1873,28 +1873,28 @@
         <v>14.0</v>
       </c>
       <c r="C7" s="0"/>
-      <c r="D7" t="n" s="93">
+      <c r="D7" t="n" s="97">
         <v>0.6428571428571429</v>
       </c>
-      <c r="E7" t="n" s="94">
+      <c r="E7" t="n" s="91">
         <v>0.14285714285714285</v>
       </c>
-      <c r="F7" t="n" s="90">
-        <v>0.0</v>
-      </c>
-      <c r="G7" t="n" s="97">
+      <c r="F7" t="n" s="92">
+        <v>0.0</v>
+      </c>
+      <c r="G7" t="n" s="95">
         <v>0.2857142857142857</v>
       </c>
-      <c r="H7" t="n" s="95">
+      <c r="H7" t="n" s="90">
         <v>0.7142857142857143</v>
       </c>
-      <c r="I7" t="n" s="92">
+      <c r="I7" t="n" s="93">
         <v>1.2142857142857142</v>
       </c>
-      <c r="J7" t="n" s="96">
-        <v>0.0</v>
-      </c>
-      <c r="K7" t="n" s="91">
+      <c r="J7" t="n" s="94">
+        <v>0.0</v>
+      </c>
+      <c r="K7" t="n" s="96">
         <v>0.5714285714285714</v>
       </c>
     </row>
@@ -1906,28 +1906,28 @@
         <v>15.0</v>
       </c>
       <c r="C8" s="0"/>
-      <c r="D8" t="n" s="117">
+      <c r="D8" t="n" s="121">
         <v>1.0666666666666667</v>
       </c>
-      <c r="E8" t="n" s="118">
+      <c r="E8" t="n" s="115">
         <v>0.06666666666666667</v>
       </c>
-      <c r="F8" t="n" s="114">
-        <v>0.0</v>
-      </c>
-      <c r="G8" t="n" s="121">
+      <c r="F8" t="n" s="116">
+        <v>0.0</v>
+      </c>
+      <c r="G8" t="n" s="119">
         <v>0.5333333333333333</v>
       </c>
-      <c r="H8" t="n" s="119">
+      <c r="H8" t="n" s="114">
         <v>0.8</v>
       </c>
-      <c r="I8" t="n" s="116">
+      <c r="I8" t="n" s="117">
         <v>1.5333333333333334</v>
       </c>
-      <c r="J8" t="n" s="120">
-        <v>0.0</v>
-      </c>
-      <c r="K8" t="n" s="115">
+      <c r="J8" t="n" s="118">
+        <v>0.0</v>
+      </c>
+      <c r="K8" t="n" s="120">
         <v>0.9333333333333333</v>
       </c>
     </row>
@@ -1939,28 +1939,28 @@
         <v>15.0</v>
       </c>
       <c r="C9" s="0"/>
-      <c r="D9" t="n" s="141">
+      <c r="D9" t="n" s="145">
         <v>0.6666666666666666</v>
       </c>
-      <c r="E9" t="n" s="142">
+      <c r="E9" t="n" s="139">
         <v>0.06666666666666667</v>
       </c>
-      <c r="F9" t="n" s="138">
-        <v>0.0</v>
-      </c>
-      <c r="G9" t="n" s="145">
+      <c r="F9" t="n" s="140">
+        <v>0.0</v>
+      </c>
+      <c r="G9" t="n" s="143">
         <v>0.3333333333333333</v>
       </c>
-      <c r="H9" t="n" s="143">
+      <c r="H9" t="n" s="138">
         <v>0.9333333333333333</v>
       </c>
-      <c r="I9" t="n" s="140">
+      <c r="I9" t="n" s="141">
         <v>1.6</v>
       </c>
-      <c r="J9" t="n" s="144">
-        <v>0.0</v>
-      </c>
-      <c r="K9" t="n" s="139">
+      <c r="J9" t="n" s="142">
+        <v>0.0</v>
+      </c>
+      <c r="K9" t="n" s="144">
         <v>0.4</v>
       </c>
     </row>
@@ -1972,28 +1972,28 @@
         <v>15.0</v>
       </c>
       <c r="C10" s="0"/>
-      <c r="D10" t="n" s="165">
+      <c r="D10" t="n" s="169">
         <v>0.8666666666666667</v>
       </c>
-      <c r="E10" t="n" s="166">
-        <v>0.0</v>
-      </c>
-      <c r="F10" t="n" s="162">
-        <v>0.0</v>
-      </c>
-      <c r="G10" t="n" s="169">
+      <c r="E10" t="n" s="163">
+        <v>0.0</v>
+      </c>
+      <c r="F10" t="n" s="164">
+        <v>0.0</v>
+      </c>
+      <c r="G10" t="n" s="167">
         <v>0.2</v>
       </c>
-      <c r="H10" t="n" s="167">
+      <c r="H10" t="n" s="162">
         <v>0.8</v>
       </c>
-      <c r="I10" t="n" s="164">
+      <c r="I10" t="n" s="165">
         <v>1.4</v>
       </c>
-      <c r="J10" t="n" s="168">
-        <v>0.0</v>
-      </c>
-      <c r="K10" t="n" s="163">
+      <c r="J10" t="n" s="166">
+        <v>0.0</v>
+      </c>
+      <c r="K10" t="n" s="168">
         <v>0.4666666666666667</v>
       </c>
     </row>
@@ -2005,28 +2005,28 @@
         <v>15.0</v>
       </c>
       <c r="C11" s="0"/>
-      <c r="D11" t="n" s="189">
+      <c r="D11" t="n" s="193">
         <v>0.6666666666666666</v>
       </c>
-      <c r="E11" t="n" s="190">
+      <c r="E11" t="n" s="187">
         <v>0.06666666666666667</v>
       </c>
-      <c r="F11" t="n" s="186">
-        <v>0.0</v>
-      </c>
-      <c r="G11" t="n" s="193">
+      <c r="F11" t="n" s="188">
+        <v>0.0</v>
+      </c>
+      <c r="G11" t="n" s="191">
         <v>0.4</v>
       </c>
-      <c r="H11" t="n" s="191">
+      <c r="H11" t="n" s="186">
         <v>1.1333333333333333</v>
       </c>
-      <c r="I11" t="n" s="188">
+      <c r="I11" t="n" s="189">
         <v>1.3333333333333333</v>
       </c>
-      <c r="J11" t="n" s="192">
+      <c r="J11" t="n" s="190">
         <v>0.13333333333333333</v>
       </c>
-      <c r="K11" t="n" s="187">
+      <c r="K11" t="n" s="192">
         <v>0.8</v>
       </c>
     </row>
@@ -2038,28 +2038,28 @@
         <v>15.0</v>
       </c>
       <c r="C12" s="0"/>
-      <c r="D12" t="n" s="213">
+      <c r="D12" t="n" s="217">
         <v>0.6</v>
       </c>
-      <c r="E12" t="n" s="214">
+      <c r="E12" t="n" s="211">
         <v>0.13333333333333333</v>
       </c>
-      <c r="F12" t="n" s="210">
-        <v>0.0</v>
-      </c>
-      <c r="G12" t="n" s="217">
+      <c r="F12" t="n" s="212">
+        <v>0.0</v>
+      </c>
+      <c r="G12" t="n" s="215">
         <v>0.2</v>
       </c>
-      <c r="H12" t="n" s="215">
+      <c r="H12" t="n" s="210">
         <v>0.8666666666666667</v>
       </c>
-      <c r="I12" t="n" s="212">
+      <c r="I12" t="n" s="213">
         <v>1.2666666666666666</v>
       </c>
-      <c r="J12" t="n" s="216">
-        <v>0.0</v>
-      </c>
-      <c r="K12" t="n" s="211">
+      <c r="J12" t="n" s="214">
+        <v>0.0</v>
+      </c>
+      <c r="K12" t="n" s="216">
         <v>0.5333333333333333</v>
       </c>
     </row>
@@ -2071,28 +2071,28 @@
         <v>15.0</v>
       </c>
       <c r="C13" s="0"/>
-      <c r="D13" t="n" s="237">
+      <c r="D13" t="n" s="241">
         <v>0.4</v>
       </c>
-      <c r="E13" t="n" s="238">
+      <c r="E13" t="n" s="235">
         <v>0.2</v>
       </c>
-      <c r="F13" t="n" s="234">
-        <v>0.0</v>
-      </c>
-      <c r="G13" t="n" s="241">
+      <c r="F13" t="n" s="236">
+        <v>0.0</v>
+      </c>
+      <c r="G13" t="n" s="239">
         <v>0.3333333333333333</v>
       </c>
-      <c r="H13" t="n" s="239">
+      <c r="H13" t="n" s="234">
         <v>0.9333333333333333</v>
       </c>
-      <c r="I13" t="n" s="236">
+      <c r="I13" t="n" s="237">
         <v>1.0</v>
       </c>
-      <c r="J13" t="n" s="240">
+      <c r="J13" t="n" s="238">
         <v>0.06666666666666667</v>
       </c>
-      <c r="K13" t="n" s="235">
+      <c r="K13" t="n" s="240">
         <v>0.8</v>
       </c>
     </row>
@@ -2104,28 +2104,28 @@
         <v>15.0</v>
       </c>
       <c r="C14" s="0"/>
-      <c r="D14" t="n" s="261">
+      <c r="D14" t="n" s="265">
         <v>0.6666666666666666</v>
       </c>
-      <c r="E14" t="n" s="262">
-        <v>0.0</v>
-      </c>
-      <c r="F14" t="n" s="258">
-        <v>0.0</v>
-      </c>
-      <c r="G14" t="n" s="265">
+      <c r="E14" t="n" s="259">
+        <v>0.0</v>
+      </c>
+      <c r="F14" t="n" s="260">
+        <v>0.0</v>
+      </c>
+      <c r="G14" t="n" s="263">
         <v>0.4666666666666667</v>
       </c>
-      <c r="H14" t="n" s="263">
+      <c r="H14" t="n" s="258">
         <v>0.8</v>
       </c>
-      <c r="I14" t="n" s="260">
+      <c r="I14" t="n" s="261">
         <v>1.1333333333333333</v>
       </c>
-      <c r="J14" t="n" s="264">
-        <v>0.0</v>
-      </c>
-      <c r="K14" t="n" s="259">
+      <c r="J14" t="n" s="262">
+        <v>0.0</v>
+      </c>
+      <c r="K14" t="n" s="264">
         <v>0.8</v>
       </c>
     </row>
@@ -2137,28 +2137,28 @@
         <v>15.0</v>
       </c>
       <c r="C15" s="0"/>
-      <c r="D15" t="n" s="285">
+      <c r="D15" t="n" s="289">
         <v>0.4666666666666667</v>
       </c>
-      <c r="E15" t="n" s="286">
-        <v>0.0</v>
-      </c>
-      <c r="F15" t="n" s="282">
-        <v>0.0</v>
-      </c>
-      <c r="G15" t="n" s="289">
+      <c r="E15" t="n" s="283">
+        <v>0.0</v>
+      </c>
+      <c r="F15" t="n" s="284">
+        <v>0.0</v>
+      </c>
+      <c r="G15" t="n" s="287">
         <v>0.4666666666666667</v>
       </c>
-      <c r="H15" t="n" s="287">
+      <c r="H15" t="n" s="282">
         <v>0.7333333333333333</v>
       </c>
-      <c r="I15" t="n" s="284">
+      <c r="I15" t="n" s="285">
         <v>1.0666666666666667</v>
       </c>
-      <c r="J15" t="n" s="288">
-        <v>0.0</v>
-      </c>
-      <c r="K15" t="n" s="283">
+      <c r="J15" t="n" s="286">
+        <v>0.0</v>
+      </c>
+      <c r="K15" t="n" s="288">
         <v>0.6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
lang phInventory checking and phCategorizing
</commit_message>
<xml_diff>
--- a/src/main/java/output/Normality.xlsx
+++ b/src/main/java/output/Normality.xlsx
@@ -40,28 +40,28 @@
     <t>Backness</t>
   </si>
   <si>
+    <t>Mid</t>
+  </si>
+  <si>
+    <t>Back</t>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>Front</t>
+  </si>
+  <si>
+    <t>Op-mid</t>
+  </si>
+  <si>
+    <t>Cent</t>
+  </si>
+  <si>
     <t>Cl-mid</t>
-  </si>
-  <si>
-    <t>Front</t>
-  </si>
-  <si>
-    <t>Cent</t>
-  </si>
-  <si>
-    <t>Close</t>
-  </si>
-  <si>
-    <t>Back</t>
-  </si>
-  <si>
-    <t>Op-mid</t>
-  </si>
-  <si>
-    <t>Open</t>
-  </si>
-  <si>
-    <t>Mid</t>
   </si>
   <si>
     <t>MANNER</t>
@@ -206,290 +206,290 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true" applyBorder="true"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="true"/>
@@ -586,28 +586,28 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>20</v>
@@ -654,28 +654,28 @@
         <v>14.0</v>
       </c>
       <c r="C4" s="0"/>
-      <c r="D4" t="n" s="8">
+      <c r="D4" t="n" s="4">
         <v>0.5</v>
       </c>
       <c r="E4" t="n" s="7">
         <v>0.0</v>
       </c>
-      <c r="F4" t="n" s="9">
+      <c r="F4" t="n" s="2">
         <v>0.07142857142857142</v>
       </c>
-      <c r="G4" t="n" s="2">
+      <c r="G4" t="n" s="9">
         <v>0.21428571428571427</v>
       </c>
       <c r="H4" t="n" s="5">
         <v>0.5</v>
       </c>
-      <c r="I4" t="n" s="3">
+      <c r="I4" t="n" s="6">
         <v>0.5714285714285714</v>
       </c>
-      <c r="J4" t="n" s="4">
+      <c r="J4" t="n" s="8">
         <v>0.21428571428571427</v>
       </c>
-      <c r="K4" t="n" s="6">
+      <c r="K4" t="n" s="3">
         <v>0.2857142857142857</v>
       </c>
     </row>
@@ -687,28 +687,28 @@
         <v>14.0</v>
       </c>
       <c r="C5" s="0"/>
-      <c r="D5" t="n" s="32">
+      <c r="D5" t="n" s="28">
         <v>0.5</v>
       </c>
       <c r="E5" t="n" s="31">
         <v>0.07142857142857142</v>
       </c>
-      <c r="F5" t="n" s="33">
-        <v>0.0</v>
-      </c>
-      <c r="G5" t="n" s="26">
+      <c r="F5" t="n" s="26">
+        <v>0.0</v>
+      </c>
+      <c r="G5" t="n" s="33">
         <v>0.2857142857142857</v>
       </c>
       <c r="H5" t="n" s="29">
         <v>0.35714285714285715</v>
       </c>
-      <c r="I5" t="n" s="27">
+      <c r="I5" t="n" s="30">
         <v>0.7857142857142857</v>
       </c>
-      <c r="J5" t="n" s="28">
+      <c r="J5" t="n" s="32">
         <v>0.14285714285714285</v>
       </c>
-      <c r="K5" t="n" s="30">
+      <c r="K5" t="n" s="27">
         <v>0.21428571428571427</v>
       </c>
     </row>
@@ -720,28 +720,28 @@
         <v>14.0</v>
       </c>
       <c r="C6" s="0"/>
-      <c r="D6" t="n" s="56">
+      <c r="D6" t="n" s="52">
         <v>0.42857142857142855</v>
       </c>
       <c r="E6" t="n" s="55">
         <v>0.07142857142857142</v>
       </c>
-      <c r="F6" t="n" s="57">
-        <v>0.0</v>
-      </c>
-      <c r="G6" t="n" s="50">
+      <c r="F6" t="n" s="50">
+        <v>0.0</v>
+      </c>
+      <c r="G6" t="n" s="57">
         <v>0.35714285714285715</v>
       </c>
       <c r="H6" t="n" s="53">
         <v>0.5714285714285714</v>
       </c>
-      <c r="I6" t="n" s="51">
+      <c r="I6" t="n" s="54">
         <v>0.6428571428571429</v>
       </c>
-      <c r="J6" t="n" s="52">
-        <v>0.0</v>
-      </c>
-      <c r="K6" t="n" s="54">
+      <c r="J6" t="n" s="56">
+        <v>0.0</v>
+      </c>
+      <c r="K6" t="n" s="51">
         <v>0.5</v>
       </c>
     </row>
@@ -753,28 +753,28 @@
         <v>13.0</v>
       </c>
       <c r="C7" s="0"/>
-      <c r="D7" t="n" s="80">
+      <c r="D7" t="n" s="76">
         <v>0.5384615384615384</v>
       </c>
       <c r="E7" t="n" s="79">
         <v>0.15384615384615385</v>
       </c>
-      <c r="F7" t="n" s="81">
-        <v>0.0</v>
-      </c>
-      <c r="G7" t="n" s="74">
+      <c r="F7" t="n" s="74">
+        <v>0.0</v>
+      </c>
+      <c r="G7" t="n" s="81">
         <v>0.3076923076923077</v>
       </c>
       <c r="H7" t="n" s="77">
         <v>0.5384615384615384</v>
       </c>
-      <c r="I7" t="n" s="75">
+      <c r="I7" t="n" s="78">
         <v>0.7692307692307693</v>
       </c>
-      <c r="J7" t="n" s="76">
-        <v>0.0</v>
-      </c>
-      <c r="K7" t="n" s="78">
+      <c r="J7" t="n" s="80">
+        <v>0.0</v>
+      </c>
+      <c r="K7" t="n" s="75">
         <v>0.5384615384615384</v>
       </c>
     </row>
@@ -786,28 +786,28 @@
         <v>14.0</v>
       </c>
       <c r="C8" s="0"/>
-      <c r="D8" t="n" s="104">
+      <c r="D8" t="n" s="100">
         <v>0.7142857142857143</v>
       </c>
       <c r="E8" t="n" s="103">
         <v>0.0</v>
       </c>
-      <c r="F8" t="n" s="105">
-        <v>0.0</v>
-      </c>
-      <c r="G8" t="n" s="98">
+      <c r="F8" t="n" s="98">
+        <v>0.0</v>
+      </c>
+      <c r="G8" t="n" s="105">
         <v>0.42857142857142855</v>
       </c>
       <c r="H8" t="n" s="101">
         <v>0.5</v>
       </c>
-      <c r="I8" t="n" s="99">
+      <c r="I8" t="n" s="102">
         <v>0.8571428571428571</v>
       </c>
-      <c r="J8" t="n" s="100">
-        <v>0.0</v>
-      </c>
-      <c r="K8" t="n" s="102">
+      <c r="J8" t="n" s="104">
+        <v>0.0</v>
+      </c>
+      <c r="K8" t="n" s="99">
         <v>0.6428571428571429</v>
       </c>
     </row>
@@ -819,28 +819,28 @@
         <v>14.0</v>
       </c>
       <c r="C9" s="0"/>
-      <c r="D9" t="n" s="128">
+      <c r="D9" t="n" s="124">
         <v>0.35714285714285715</v>
       </c>
       <c r="E9" t="n" s="127">
         <v>0.07142857142857142</v>
       </c>
-      <c r="F9" t="n" s="129">
-        <v>0.0</v>
-      </c>
-      <c r="G9" t="n" s="122">
+      <c r="F9" t="n" s="122">
+        <v>0.0</v>
+      </c>
+      <c r="G9" t="n" s="129">
         <v>0.2857142857142857</v>
       </c>
       <c r="H9" t="n" s="125">
         <v>0.6428571428571429</v>
       </c>
-      <c r="I9" t="n" s="123">
+      <c r="I9" t="n" s="126">
         <v>0.7857142857142857</v>
       </c>
-      <c r="J9" t="n" s="124">
-        <v>0.0</v>
-      </c>
-      <c r="K9" t="n" s="126">
+      <c r="J9" t="n" s="128">
+        <v>0.0</v>
+      </c>
+      <c r="K9" t="n" s="123">
         <v>0.2857142857142857</v>
       </c>
     </row>
@@ -852,28 +852,28 @@
         <v>14.0</v>
       </c>
       <c r="C10" s="0"/>
-      <c r="D10" t="n" s="152">
+      <c r="D10" t="n" s="148">
         <v>0.5714285714285714</v>
       </c>
       <c r="E10" t="n" s="151">
         <v>0.0</v>
       </c>
-      <c r="F10" t="n" s="153">
-        <v>0.0</v>
-      </c>
-      <c r="G10" t="n" s="146">
+      <c r="F10" t="n" s="146">
+        <v>0.0</v>
+      </c>
+      <c r="G10" t="n" s="153">
         <v>0.21428571428571427</v>
       </c>
       <c r="H10" t="n" s="149">
         <v>0.7142857142857143</v>
       </c>
-      <c r="I10" t="n" s="147">
+      <c r="I10" t="n" s="150">
         <v>1.0</v>
       </c>
-      <c r="J10" t="n" s="148">
-        <v>0.0</v>
-      </c>
-      <c r="K10" t="n" s="150">
+      <c r="J10" t="n" s="152">
+        <v>0.0</v>
+      </c>
+      <c r="K10" t="n" s="147">
         <v>0.5</v>
       </c>
     </row>
@@ -885,28 +885,28 @@
         <v>14.0</v>
       </c>
       <c r="C11" s="0"/>
-      <c r="D11" t="n" s="176">
+      <c r="D11" t="n" s="172">
         <v>0.5</v>
       </c>
       <c r="E11" t="n" s="175">
         <v>0.07142857142857142</v>
       </c>
-      <c r="F11" t="n" s="177">
-        <v>0.0</v>
-      </c>
-      <c r="G11" t="n" s="170">
+      <c r="F11" t="n" s="170">
+        <v>0.0</v>
+      </c>
+      <c r="G11" t="n" s="177">
         <v>0.14285714285714285</v>
       </c>
       <c r="H11" t="n" s="173">
         <v>0.7142857142857143</v>
       </c>
-      <c r="I11" t="n" s="171">
+      <c r="I11" t="n" s="174">
         <v>0.7142857142857143</v>
       </c>
-      <c r="J11" t="n" s="172">
+      <c r="J11" t="n" s="176">
         <v>0.14285714285714285</v>
       </c>
-      <c r="K11" t="n" s="174">
+      <c r="K11" t="n" s="171">
         <v>0.5714285714285714</v>
       </c>
     </row>
@@ -918,28 +918,28 @@
         <v>14.0</v>
       </c>
       <c r="C12" s="0"/>
-      <c r="D12" t="n" s="200">
+      <c r="D12" t="n" s="196">
         <v>0.42857142857142855</v>
       </c>
       <c r="E12" t="n" s="199">
         <v>0.07142857142857142</v>
       </c>
-      <c r="F12" t="n" s="201">
-        <v>0.0</v>
-      </c>
-      <c r="G12" t="n" s="194">
+      <c r="F12" t="n" s="194">
+        <v>0.0</v>
+      </c>
+      <c r="G12" t="n" s="201">
         <v>0.21428571428571427</v>
       </c>
       <c r="H12" t="n" s="197">
         <v>0.7857142857142857</v>
       </c>
-      <c r="I12" t="n" s="195">
+      <c r="I12" t="n" s="198">
         <v>0.7142857142857143</v>
       </c>
-      <c r="J12" t="n" s="196">
-        <v>0.0</v>
-      </c>
-      <c r="K12" t="n" s="198">
+      <c r="J12" t="n" s="200">
+        <v>0.0</v>
+      </c>
+      <c r="K12" t="n" s="195">
         <v>0.42857142857142855</v>
       </c>
     </row>
@@ -951,28 +951,28 @@
         <v>14.0</v>
       </c>
       <c r="C13" s="0"/>
-      <c r="D13" t="n" s="224">
+      <c r="D13" t="n" s="220">
         <v>0.21428571428571427</v>
       </c>
       <c r="E13" t="n" s="223">
         <v>0.14285714285714285</v>
       </c>
-      <c r="F13" t="n" s="225">
-        <v>0.0</v>
-      </c>
-      <c r="G13" t="n" s="218">
+      <c r="F13" t="n" s="218">
+        <v>0.0</v>
+      </c>
+      <c r="G13" t="n" s="225">
         <v>0.2857142857142857</v>
       </c>
       <c r="H13" t="n" s="221">
         <v>0.5714285714285714</v>
       </c>
-      <c r="I13" t="n" s="219">
+      <c r="I13" t="n" s="222">
         <v>0.5</v>
       </c>
-      <c r="J13" t="n" s="220">
+      <c r="J13" t="n" s="224">
         <v>0.07142857142857142</v>
       </c>
-      <c r="K13" t="n" s="222">
+      <c r="K13" t="n" s="219">
         <v>0.6428571428571429</v>
       </c>
     </row>
@@ -984,28 +984,28 @@
         <v>14.0</v>
       </c>
       <c r="C14" s="0"/>
-      <c r="D14" t="n" s="248">
+      <c r="D14" t="n" s="244">
         <v>0.35714285714285715</v>
       </c>
       <c r="E14" t="n" s="247">
         <v>0.0</v>
       </c>
-      <c r="F14" t="n" s="249">
-        <v>0.0</v>
-      </c>
-      <c r="G14" t="n" s="242">
+      <c r="F14" t="n" s="242">
+        <v>0.0</v>
+      </c>
+      <c r="G14" t="n" s="249">
         <v>0.42857142857142855</v>
       </c>
       <c r="H14" t="n" s="245">
         <v>0.5714285714285714</v>
       </c>
-      <c r="I14" t="n" s="243">
+      <c r="I14" t="n" s="246">
         <v>0.6428571428571429</v>
       </c>
-      <c r="J14" t="n" s="244">
-        <v>0.0</v>
-      </c>
-      <c r="K14" t="n" s="246">
+      <c r="J14" t="n" s="248">
+        <v>0.0</v>
+      </c>
+      <c r="K14" t="n" s="243">
         <v>0.6428571428571429</v>
       </c>
     </row>
@@ -1017,28 +1017,28 @@
         <v>14.0</v>
       </c>
       <c r="C15" s="0"/>
-      <c r="D15" t="n" s="272">
+      <c r="D15" t="n" s="268">
         <v>0.2857142857142857</v>
       </c>
       <c r="E15" t="n" s="271">
         <v>0.0</v>
       </c>
-      <c r="F15" t="n" s="273">
-        <v>0.0</v>
-      </c>
-      <c r="G15" t="n" s="266">
+      <c r="F15" t="n" s="266">
+        <v>0.0</v>
+      </c>
+      <c r="G15" t="n" s="273">
         <v>0.42857142857142855</v>
       </c>
       <c r="H15" t="n" s="269">
         <v>0.35714285714285715</v>
       </c>
-      <c r="I15" t="n" s="267">
+      <c r="I15" t="n" s="270">
         <v>0.5</v>
       </c>
-      <c r="J15" t="n" s="268">
-        <v>0.0</v>
-      </c>
-      <c r="K15" t="n" s="270">
+      <c r="J15" t="n" s="272">
+        <v>0.0</v>
+      </c>
+      <c r="K15" t="n" s="267">
         <v>0.5714285714285714</v>
       </c>
     </row>
@@ -1146,28 +1146,28 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>20</v>
@@ -1214,28 +1214,28 @@
         <v>14.0</v>
       </c>
       <c r="C4" s="0"/>
-      <c r="D4" t="n" s="16">
+      <c r="D4" t="n" s="12">
         <v>0.11764705882352941</v>
       </c>
       <c r="E4" t="n" s="15">
         <v>0.0</v>
       </c>
-      <c r="F4" t="n" s="17">
+      <c r="F4" t="n" s="10">
         <v>0.014705882352941176</v>
       </c>
-      <c r="G4" t="n" s="10">
+      <c r="G4" t="n" s="17">
         <v>0.04411764705882353</v>
       </c>
       <c r="H4" t="n" s="13">
         <v>0.1323529411764706</v>
       </c>
-      <c r="I4" t="n" s="11">
+      <c r="I4" t="n" s="14">
         <v>0.16176470588235295</v>
       </c>
-      <c r="J4" t="n" s="12">
+      <c r="J4" t="n" s="16">
         <v>0.04411764705882353</v>
       </c>
-      <c r="K4" t="n" s="14">
+      <c r="K4" t="n" s="11">
         <v>0.10294117647058823</v>
       </c>
     </row>
@@ -1247,28 +1247,28 @@
         <v>14.0</v>
       </c>
       <c r="C5" s="0"/>
-      <c r="D5" t="n" s="40">
+      <c r="D5" t="n" s="36">
         <v>0.1267605633802817</v>
       </c>
       <c r="E5" t="n" s="39">
         <v>0.014084507042253521</v>
       </c>
-      <c r="F5" t="n" s="41">
-        <v>0.0</v>
-      </c>
-      <c r="G5" t="n" s="34">
+      <c r="F5" t="n" s="34">
+        <v>0.0</v>
+      </c>
+      <c r="G5" t="n" s="41">
         <v>0.08450704225352113</v>
       </c>
       <c r="H5" t="n" s="37">
         <v>0.08450704225352113</v>
       </c>
-      <c r="I5" t="n" s="35">
+      <c r="I5" t="n" s="38">
         <v>0.23943661971830985</v>
       </c>
-      <c r="J5" t="n" s="36">
+      <c r="J5" t="n" s="40">
         <v>0.028169014084507043</v>
       </c>
-      <c r="K5" t="n" s="38">
+      <c r="K5" t="n" s="35">
         <v>0.04225352112676056</v>
       </c>
     </row>
@@ -1280,28 +1280,28 @@
         <v>14.0</v>
       </c>
       <c r="C6" s="0"/>
-      <c r="D6" t="n" s="64">
+      <c r="D6" t="n" s="60">
         <v>0.11290322580645161</v>
       </c>
       <c r="E6" t="n" s="63">
         <v>0.016129032258064516</v>
       </c>
-      <c r="F6" t="n" s="65">
-        <v>0.0</v>
-      </c>
-      <c r="G6" t="n" s="58">
+      <c r="F6" t="n" s="58">
+        <v>0.0</v>
+      </c>
+      <c r="G6" t="n" s="65">
         <v>0.08064516129032258</v>
       </c>
       <c r="H6" t="n" s="61">
         <v>0.16129032258064516</v>
       </c>
-      <c r="I6" t="n" s="59">
+      <c r="I6" t="n" s="62">
         <v>0.24193548387096775</v>
       </c>
-      <c r="J6" t="n" s="60">
-        <v>0.0</v>
-      </c>
-      <c r="K6" t="n" s="62">
+      <c r="J6" t="n" s="64">
+        <v>0.0</v>
+      </c>
+      <c r="K6" t="n" s="59">
         <v>0.12903225806451613</v>
       </c>
     </row>
@@ -1313,28 +1313,28 @@
         <v>13.0</v>
       </c>
       <c r="C7" s="0"/>
-      <c r="D7" t="n" s="88">
+      <c r="D7" t="n" s="84">
         <v>0.1095890410958904</v>
       </c>
       <c r="E7" t="n" s="87">
         <v>0.0273972602739726</v>
       </c>
-      <c r="F7" t="n" s="89">
-        <v>0.0</v>
-      </c>
-      <c r="G7" t="n" s="82">
+      <c r="F7" t="n" s="82">
+        <v>0.0</v>
+      </c>
+      <c r="G7" t="n" s="89">
         <v>0.0547945205479452</v>
       </c>
       <c r="H7" t="n" s="85">
         <v>0.136986301369863</v>
       </c>
-      <c r="I7" t="n" s="83">
+      <c r="I7" t="n" s="86">
         <v>0.2191780821917808</v>
       </c>
-      <c r="J7" t="n" s="84">
-        <v>0.0</v>
-      </c>
-      <c r="K7" t="n" s="86">
+      <c r="J7" t="n" s="88">
+        <v>0.0</v>
+      </c>
+      <c r="K7" t="n" s="83">
         <v>0.1095890410958904</v>
       </c>
     </row>
@@ -1346,28 +1346,28 @@
         <v>14.0</v>
       </c>
       <c r="C8" s="0"/>
-      <c r="D8" t="n" s="112">
+      <c r="D8" t="n" s="108">
         <v>0.18292682926829268</v>
       </c>
       <c r="E8" t="n" s="111">
         <v>0.0</v>
       </c>
-      <c r="F8" t="n" s="113">
-        <v>0.0</v>
-      </c>
-      <c r="G8" t="n" s="106">
+      <c r="F8" t="n" s="106">
+        <v>0.0</v>
+      </c>
+      <c r="G8" t="n" s="113">
         <v>0.0975609756097561</v>
       </c>
       <c r="H8" t="n" s="109">
         <v>0.12195121951219512</v>
       </c>
-      <c r="I8" t="n" s="107">
+      <c r="I8" t="n" s="110">
         <v>0.25609756097560976</v>
       </c>
-      <c r="J8" t="n" s="108">
-        <v>0.0</v>
-      </c>
-      <c r="K8" t="n" s="110">
+      <c r="J8" t="n" s="112">
+        <v>0.0</v>
+      </c>
+      <c r="K8" t="n" s="107">
         <v>0.14634146341463414</v>
       </c>
     </row>
@@ -1379,28 +1379,28 @@
         <v>14.0</v>
       </c>
       <c r="C9" s="0"/>
-      <c r="D9" t="n" s="136">
+      <c r="D9" t="n" s="132">
         <v>0.12121212121212122</v>
       </c>
       <c r="E9" t="n" s="135">
         <v>0.015151515151515152</v>
       </c>
-      <c r="F9" t="n" s="137">
-        <v>0.0</v>
-      </c>
-      <c r="G9" t="n" s="130">
+      <c r="F9" t="n" s="130">
+        <v>0.0</v>
+      </c>
+      <c r="G9" t="n" s="137">
         <v>0.07575757575757576</v>
       </c>
       <c r="H9" t="n" s="133">
         <v>0.19696969696969696</v>
       </c>
-      <c r="I9" t="n" s="131">
+      <c r="I9" t="n" s="134">
         <v>0.3181818181818182</v>
       </c>
-      <c r="J9" t="n" s="132">
-        <v>0.0</v>
-      </c>
-      <c r="K9" t="n" s="134">
+      <c r="J9" t="n" s="136">
+        <v>0.0</v>
+      </c>
+      <c r="K9" t="n" s="131">
         <v>0.09090909090909091</v>
       </c>
     </row>
@@ -1412,28 +1412,28 @@
         <v>14.0</v>
       </c>
       <c r="C10" s="0"/>
-      <c r="D10" t="n" s="160">
+      <c r="D10" t="n" s="156">
         <v>0.17647058823529413</v>
       </c>
       <c r="E10" t="n" s="159">
         <v>0.0</v>
       </c>
-      <c r="F10" t="n" s="161">
-        <v>0.0</v>
-      </c>
-      <c r="G10" t="n" s="154">
+      <c r="F10" t="n" s="154">
+        <v>0.0</v>
+      </c>
+      <c r="G10" t="n" s="161">
         <v>0.04411764705882353</v>
       </c>
       <c r="H10" t="n" s="157">
         <v>0.17647058823529413</v>
       </c>
-      <c r="I10" t="n" s="155">
+      <c r="I10" t="n" s="158">
         <v>0.29411764705882354</v>
       </c>
-      <c r="J10" t="n" s="156">
-        <v>0.0</v>
-      </c>
-      <c r="K10" t="n" s="158">
+      <c r="J10" t="n" s="160">
+        <v>0.0</v>
+      </c>
+      <c r="K10" t="n" s="155">
         <v>0.10294117647058823</v>
       </c>
     </row>
@@ -1445,28 +1445,28 @@
         <v>14.0</v>
       </c>
       <c r="C11" s="0"/>
-      <c r="D11" t="n" s="184">
+      <c r="D11" t="n" s="180">
         <v>0.10465116279069768</v>
       </c>
       <c r="E11" t="n" s="183">
         <v>0.011627906976744186</v>
       </c>
-      <c r="F11" t="n" s="185">
-        <v>0.0</v>
-      </c>
-      <c r="G11" t="n" s="178">
+      <c r="F11" t="n" s="178">
+        <v>0.0</v>
+      </c>
+      <c r="G11" t="n" s="185">
         <v>0.05813953488372093</v>
       </c>
       <c r="H11" t="n" s="181">
         <v>0.18604651162790697</v>
       </c>
-      <c r="I11" t="n" s="179">
+      <c r="I11" t="n" s="182">
         <v>0.19767441860465115</v>
       </c>
-      <c r="J11" t="n" s="180">
+      <c r="J11" t="n" s="184">
         <v>0.023255813953488372</v>
       </c>
-      <c r="K11" t="n" s="182">
+      <c r="K11" t="n" s="179">
         <v>0.13953488372093023</v>
       </c>
     </row>
@@ -1478,28 +1478,28 @@
         <v>14.0</v>
       </c>
       <c r="C12" s="0"/>
-      <c r="D12" t="n" s="208">
+      <c r="D12" t="n" s="204">
         <v>0.12698412698412698</v>
       </c>
       <c r="E12" t="n" s="207">
         <v>0.015873015873015872</v>
       </c>
-      <c r="F12" t="n" s="209">
-        <v>0.0</v>
-      </c>
-      <c r="G12" t="n" s="202">
+      <c r="F12" t="n" s="202">
+        <v>0.0</v>
+      </c>
+      <c r="G12" t="n" s="209">
         <v>0.047619047619047616</v>
       </c>
       <c r="H12" t="n" s="205">
         <v>0.20634920634920634</v>
       </c>
-      <c r="I12" t="n" s="203">
+      <c r="I12" t="n" s="206">
         <v>0.2698412698412698</v>
       </c>
-      <c r="J12" t="n" s="204">
-        <v>0.0</v>
-      </c>
-      <c r="K12" t="n" s="206">
+      <c r="J12" t="n" s="208">
+        <v>0.0</v>
+      </c>
+      <c r="K12" t="n" s="203">
         <v>0.12698412698412698</v>
       </c>
     </row>
@@ -1511,28 +1511,28 @@
         <v>14.0</v>
       </c>
       <c r="C13" s="0"/>
-      <c r="D13" t="n" s="232">
+      <c r="D13" t="n" s="228">
         <v>0.06349206349206349</v>
       </c>
       <c r="E13" t="n" s="231">
         <v>0.031746031746031744</v>
       </c>
-      <c r="F13" t="n" s="233">
-        <v>0.0</v>
-      </c>
-      <c r="G13" t="n" s="226">
+      <c r="F13" t="n" s="226">
+        <v>0.0</v>
+      </c>
+      <c r="G13" t="n" s="233">
         <v>0.07936507936507936</v>
       </c>
       <c r="H13" t="n" s="229">
         <v>0.2222222222222222</v>
       </c>
-      <c r="I13" t="n" s="227">
+      <c r="I13" t="n" s="230">
         <v>0.20634920634920634</v>
       </c>
-      <c r="J13" t="n" s="228">
+      <c r="J13" t="n" s="232">
         <v>0.015873015873015872</v>
       </c>
-      <c r="K13" t="n" s="230">
+      <c r="K13" t="n" s="227">
         <v>0.1746031746031746</v>
       </c>
     </row>
@@ -1544,28 +1544,28 @@
         <v>14.0</v>
       </c>
       <c r="C14" s="0"/>
-      <c r="D14" t="n" s="256">
+      <c r="D14" t="n" s="252">
         <v>0.125</v>
       </c>
       <c r="E14" t="n" s="255">
         <v>0.0</v>
       </c>
-      <c r="F14" t="n" s="257">
-        <v>0.0</v>
-      </c>
-      <c r="G14" t="n" s="250">
+      <c r="F14" t="n" s="250">
+        <v>0.0</v>
+      </c>
+      <c r="G14" t="n" s="257">
         <v>0.09722222222222222</v>
       </c>
       <c r="H14" t="n" s="253">
         <v>0.1388888888888889</v>
       </c>
-      <c r="I14" t="n" s="251">
+      <c r="I14" t="n" s="254">
         <v>0.2222222222222222</v>
       </c>
-      <c r="J14" t="n" s="252">
-        <v>0.0</v>
-      </c>
-      <c r="K14" t="n" s="254">
+      <c r="J14" t="n" s="256">
+        <v>0.0</v>
+      </c>
+      <c r="K14" t="n" s="251">
         <v>0.1388888888888889</v>
       </c>
     </row>
@@ -1577,28 +1577,28 @@
         <v>14.0</v>
       </c>
       <c r="C15" s="0"/>
-      <c r="D15" t="n" s="280">
+      <c r="D15" t="n" s="276">
         <v>0.08928571428571429</v>
       </c>
       <c r="E15" t="n" s="279">
         <v>0.0</v>
       </c>
-      <c r="F15" t="n" s="281">
-        <v>0.0</v>
-      </c>
-      <c r="G15" t="n" s="274">
+      <c r="F15" t="n" s="274">
+        <v>0.0</v>
+      </c>
+      <c r="G15" t="n" s="281">
         <v>0.125</v>
       </c>
       <c r="H15" t="n" s="277">
         <v>0.16071428571428573</v>
       </c>
-      <c r="I15" t="n" s="275">
+      <c r="I15" t="n" s="278">
         <v>0.21428571428571427</v>
       </c>
-      <c r="J15" t="n" s="276">
-        <v>0.0</v>
-      </c>
-      <c r="K15" t="n" s="278">
+      <c r="J15" t="n" s="280">
+        <v>0.0</v>
+      </c>
+      <c r="K15" t="n" s="275">
         <v>0.16071428571428573</v>
       </c>
     </row>
@@ -1706,28 +1706,28 @@
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
       <c r="D3" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>8</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>11</v>
       </c>
       <c r="I3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="1" t="s">
         <v>9</v>
-      </c>
-      <c r="J3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>12</v>
       </c>
       <c r="L3" s="1" t="s">
         <v>20</v>
@@ -1774,28 +1774,28 @@
         <v>14.0</v>
       </c>
       <c r="C4" s="0"/>
-      <c r="D4" t="n" s="24">
+      <c r="D4" t="n" s="20">
         <v>0.5714285714285714</v>
       </c>
       <c r="E4" t="n" s="23">
         <v>0.0</v>
       </c>
-      <c r="F4" t="n" s="25">
+      <c r="F4" t="n" s="18">
         <v>0.07142857142857142</v>
       </c>
-      <c r="G4" t="n" s="18">
+      <c r="G4" t="n" s="25">
         <v>0.21428571428571427</v>
       </c>
       <c r="H4" t="n" s="21">
         <v>0.6428571428571429</v>
       </c>
-      <c r="I4" t="n" s="19">
+      <c r="I4" t="n" s="22">
         <v>0.7857142857142857</v>
       </c>
-      <c r="J4" t="n" s="20">
+      <c r="J4" t="n" s="24">
         <v>0.21428571428571427</v>
       </c>
-      <c r="K4" t="n" s="22">
+      <c r="K4" t="n" s="19">
         <v>0.5</v>
       </c>
     </row>
@@ -1807,28 +1807,28 @@
         <v>14.0</v>
       </c>
       <c r="C5" s="0"/>
-      <c r="D5" t="n" s="48">
+      <c r="D5" t="n" s="44">
         <v>0.6428571428571429</v>
       </c>
       <c r="E5" t="n" s="47">
         <v>0.07142857142857142</v>
       </c>
-      <c r="F5" t="n" s="49">
-        <v>0.0</v>
-      </c>
-      <c r="G5" t="n" s="42">
+      <c r="F5" t="n" s="42">
+        <v>0.0</v>
+      </c>
+      <c r="G5" t="n" s="49">
         <v>0.42857142857142855</v>
       </c>
       <c r="H5" t="n" s="45">
         <v>0.42857142857142855</v>
       </c>
-      <c r="I5" t="n" s="43">
+      <c r="I5" t="n" s="46">
         <v>1.2142857142857142</v>
       </c>
-      <c r="J5" t="n" s="44">
+      <c r="J5" t="n" s="48">
         <v>0.14285714285714285</v>
       </c>
-      <c r="K5" t="n" s="46">
+      <c r="K5" t="n" s="43">
         <v>0.21428571428571427</v>
       </c>
     </row>
@@ -1840,28 +1840,28 @@
         <v>14.0</v>
       </c>
       <c r="C6" s="0"/>
-      <c r="D6" t="n" s="72">
+      <c r="D6" t="n" s="68">
         <v>0.5</v>
       </c>
       <c r="E6" t="n" s="71">
         <v>0.07142857142857142</v>
       </c>
-      <c r="F6" t="n" s="73">
-        <v>0.0</v>
-      </c>
-      <c r="G6" t="n" s="66">
+      <c r="F6" t="n" s="66">
+        <v>0.0</v>
+      </c>
+      <c r="G6" t="n" s="73">
         <v>0.35714285714285715</v>
       </c>
       <c r="H6" t="n" s="69">
         <v>0.7142857142857143</v>
       </c>
-      <c r="I6" t="n" s="67">
+      <c r="I6" t="n" s="70">
         <v>1.0714285714285714</v>
       </c>
-      <c r="J6" t="n" s="68">
-        <v>0.0</v>
-      </c>
-      <c r="K6" t="n" s="70">
+      <c r="J6" t="n" s="72">
+        <v>0.0</v>
+      </c>
+      <c r="K6" t="n" s="67">
         <v>0.5714285714285714</v>
       </c>
     </row>
@@ -1873,28 +1873,28 @@
         <v>13.0</v>
       </c>
       <c r="C7" s="0"/>
-      <c r="D7" t="n" s="96">
+      <c r="D7" t="n" s="92">
         <v>0.6153846153846154</v>
       </c>
       <c r="E7" t="n" s="95">
         <v>0.15384615384615385</v>
       </c>
-      <c r="F7" t="n" s="97">
-        <v>0.0</v>
-      </c>
-      <c r="G7" t="n" s="90">
+      <c r="F7" t="n" s="90">
+        <v>0.0</v>
+      </c>
+      <c r="G7" t="n" s="97">
         <v>0.3076923076923077</v>
       </c>
       <c r="H7" t="n" s="93">
         <v>0.7692307692307693</v>
       </c>
-      <c r="I7" t="n" s="91">
+      <c r="I7" t="n" s="94">
         <v>1.2307692307692308</v>
       </c>
-      <c r="J7" t="n" s="92">
-        <v>0.0</v>
-      </c>
-      <c r="K7" t="n" s="94">
+      <c r="J7" t="n" s="96">
+        <v>0.0</v>
+      </c>
+      <c r="K7" t="n" s="91">
         <v>0.6153846153846154</v>
       </c>
     </row>
@@ -1906,28 +1906,28 @@
         <v>14.0</v>
       </c>
       <c r="C8" s="0"/>
-      <c r="D8" t="n" s="120">
+      <c r="D8" t="n" s="116">
         <v>1.0714285714285714</v>
       </c>
       <c r="E8" t="n" s="119">
         <v>0.0</v>
       </c>
-      <c r="F8" t="n" s="121">
-        <v>0.0</v>
-      </c>
-      <c r="G8" t="n" s="114">
+      <c r="F8" t="n" s="114">
+        <v>0.0</v>
+      </c>
+      <c r="G8" t="n" s="121">
         <v>0.5714285714285714</v>
       </c>
       <c r="H8" t="n" s="117">
         <v>0.7142857142857143</v>
       </c>
-      <c r="I8" t="n" s="115">
+      <c r="I8" t="n" s="118">
         <v>1.5</v>
       </c>
-      <c r="J8" t="n" s="116">
-        <v>0.0</v>
-      </c>
-      <c r="K8" t="n" s="118">
+      <c r="J8" t="n" s="120">
+        <v>0.0</v>
+      </c>
+      <c r="K8" t="n" s="115">
         <v>0.8571428571428571</v>
       </c>
     </row>
@@ -1939,28 +1939,28 @@
         <v>14.0</v>
       </c>
       <c r="C9" s="0"/>
-      <c r="D9" t="n" s="144">
+      <c r="D9" t="n" s="140">
         <v>0.5714285714285714</v>
       </c>
       <c r="E9" t="n" s="143">
         <v>0.07142857142857142</v>
       </c>
-      <c r="F9" t="n" s="145">
-        <v>0.0</v>
-      </c>
-      <c r="G9" t="n" s="138">
+      <c r="F9" t="n" s="138">
+        <v>0.0</v>
+      </c>
+      <c r="G9" t="n" s="145">
         <v>0.35714285714285715</v>
       </c>
       <c r="H9" t="n" s="141">
         <v>0.9285714285714286</v>
       </c>
-      <c r="I9" t="n" s="139">
+      <c r="I9" t="n" s="142">
         <v>1.5</v>
       </c>
-      <c r="J9" t="n" s="140">
-        <v>0.0</v>
-      </c>
-      <c r="K9" t="n" s="142">
+      <c r="J9" t="n" s="144">
+        <v>0.0</v>
+      </c>
+      <c r="K9" t="n" s="139">
         <v>0.42857142857142855</v>
       </c>
     </row>
@@ -1972,28 +1972,28 @@
         <v>14.0</v>
       </c>
       <c r="C10" s="0"/>
-      <c r="D10" t="n" s="168">
+      <c r="D10" t="n" s="164">
         <v>0.8571428571428571</v>
       </c>
       <c r="E10" t="n" s="167">
         <v>0.0</v>
       </c>
-      <c r="F10" t="n" s="169">
-        <v>0.0</v>
-      </c>
-      <c r="G10" t="n" s="162">
+      <c r="F10" t="n" s="162">
+        <v>0.0</v>
+      </c>
+      <c r="G10" t="n" s="169">
         <v>0.21428571428571427</v>
       </c>
       <c r="H10" t="n" s="165">
         <v>0.8571428571428571</v>
       </c>
-      <c r="I10" t="n" s="163">
+      <c r="I10" t="n" s="166">
         <v>1.4285714285714286</v>
       </c>
-      <c r="J10" t="n" s="164">
-        <v>0.0</v>
-      </c>
-      <c r="K10" t="n" s="166">
+      <c r="J10" t="n" s="168">
+        <v>0.0</v>
+      </c>
+      <c r="K10" t="n" s="163">
         <v>0.5</v>
       </c>
     </row>
@@ -2005,28 +2005,28 @@
         <v>14.0</v>
       </c>
       <c r="C11" s="0"/>
-      <c r="D11" t="n" s="192">
+      <c r="D11" t="n" s="188">
         <v>0.6428571428571429</v>
       </c>
       <c r="E11" t="n" s="191">
         <v>0.07142857142857142</v>
       </c>
-      <c r="F11" t="n" s="193">
-        <v>0.0</v>
-      </c>
-      <c r="G11" t="n" s="186">
+      <c r="F11" t="n" s="186">
+        <v>0.0</v>
+      </c>
+      <c r="G11" t="n" s="193">
         <v>0.35714285714285715</v>
       </c>
       <c r="H11" t="n" s="189">
         <v>1.1428571428571428</v>
       </c>
-      <c r="I11" t="n" s="187">
+      <c r="I11" t="n" s="190">
         <v>1.2142857142857142</v>
       </c>
-      <c r="J11" t="n" s="188">
+      <c r="J11" t="n" s="192">
         <v>0.14285714285714285</v>
       </c>
-      <c r="K11" t="n" s="190">
+      <c r="K11" t="n" s="187">
         <v>0.8571428571428571</v>
       </c>
     </row>
@@ -2038,28 +2038,28 @@
         <v>14.0</v>
       </c>
       <c r="C12" s="0"/>
-      <c r="D12" t="n" s="216">
+      <c r="D12" t="n" s="212">
         <v>0.5714285714285714</v>
       </c>
       <c r="E12" t="n" s="215">
         <v>0.07142857142857142</v>
       </c>
-      <c r="F12" t="n" s="217">
-        <v>0.0</v>
-      </c>
-      <c r="G12" t="n" s="210">
+      <c r="F12" t="n" s="210">
+        <v>0.0</v>
+      </c>
+      <c r="G12" t="n" s="217">
         <v>0.21428571428571427</v>
       </c>
       <c r="H12" t="n" s="213">
         <v>0.9285714285714286</v>
       </c>
-      <c r="I12" t="n" s="211">
+      <c r="I12" t="n" s="214">
         <v>1.2142857142857142</v>
       </c>
-      <c r="J12" t="n" s="212">
-        <v>0.0</v>
-      </c>
-      <c r="K12" t="n" s="214">
+      <c r="J12" t="n" s="216">
+        <v>0.0</v>
+      </c>
+      <c r="K12" t="n" s="211">
         <v>0.5714285714285714</v>
       </c>
     </row>
@@ -2071,28 +2071,28 @@
         <v>14.0</v>
       </c>
       <c r="C13" s="0"/>
-      <c r="D13" t="n" s="240">
+      <c r="D13" t="n" s="236">
         <v>0.2857142857142857</v>
       </c>
       <c r="E13" t="n" s="239">
         <v>0.14285714285714285</v>
       </c>
-      <c r="F13" t="n" s="241">
-        <v>0.0</v>
-      </c>
-      <c r="G13" t="n" s="234">
+      <c r="F13" t="n" s="234">
+        <v>0.0</v>
+      </c>
+      <c r="G13" t="n" s="241">
         <v>0.35714285714285715</v>
       </c>
       <c r="H13" t="n" s="237">
         <v>1.0</v>
       </c>
-      <c r="I13" t="n" s="235">
+      <c r="I13" t="n" s="238">
         <v>0.9285714285714286</v>
       </c>
-      <c r="J13" t="n" s="236">
+      <c r="J13" t="n" s="240">
         <v>0.07142857142857142</v>
       </c>
-      <c r="K13" t="n" s="238">
+      <c r="K13" t="n" s="235">
         <v>0.7857142857142857</v>
       </c>
     </row>
@@ -2104,28 +2104,28 @@
         <v>14.0</v>
       </c>
       <c r="C14" s="0"/>
-      <c r="D14" t="n" s="264">
+      <c r="D14" t="n" s="260">
         <v>0.6428571428571429</v>
       </c>
       <c r="E14" t="n" s="263">
         <v>0.0</v>
       </c>
-      <c r="F14" t="n" s="265">
-        <v>0.0</v>
-      </c>
-      <c r="G14" t="n" s="258">
+      <c r="F14" t="n" s="258">
+        <v>0.0</v>
+      </c>
+      <c r="G14" t="n" s="265">
         <v>0.5</v>
       </c>
       <c r="H14" t="n" s="261">
         <v>0.7142857142857143</v>
       </c>
-      <c r="I14" t="n" s="259">
+      <c r="I14" t="n" s="262">
         <v>1.1428571428571428</v>
       </c>
-      <c r="J14" t="n" s="260">
-        <v>0.0</v>
-      </c>
-      <c r="K14" t="n" s="262">
+      <c r="J14" t="n" s="264">
+        <v>0.0</v>
+      </c>
+      <c r="K14" t="n" s="259">
         <v>0.7142857142857143</v>
       </c>
     </row>
@@ -2137,28 +2137,28 @@
         <v>14.0</v>
       </c>
       <c r="C15" s="0"/>
-      <c r="D15" t="n" s="288">
+      <c r="D15" t="n" s="284">
         <v>0.35714285714285715</v>
       </c>
       <c r="E15" t="n" s="287">
         <v>0.0</v>
       </c>
-      <c r="F15" t="n" s="289">
-        <v>0.0</v>
-      </c>
-      <c r="G15" t="n" s="282">
+      <c r="F15" t="n" s="282">
+        <v>0.0</v>
+      </c>
+      <c r="G15" t="n" s="289">
         <v>0.5</v>
       </c>
       <c r="H15" t="n" s="285">
         <v>0.6428571428571429</v>
       </c>
-      <c r="I15" t="n" s="283">
+      <c r="I15" t="n" s="286">
         <v>0.8571428571428571</v>
       </c>
-      <c r="J15" t="n" s="284">
-        <v>0.0</v>
-      </c>
-      <c r="K15" t="n" s="286">
+      <c r="J15" t="n" s="288">
+        <v>0.0</v>
+      </c>
+      <c r="K15" t="n" s="283">
         <v>0.6428571428571429</v>
       </c>
     </row>

</xml_diff>

<commit_message>
consonants manner in progress
</commit_message>
<xml_diff>
--- a/src/main/java/output/Normality.xlsx
+++ b/src/main/java/output/Normality.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="194">
   <si>
     <t>Semantics</t>
   </si>
@@ -88,42 +88,6 @@
     <t>Obstruent</t>
   </si>
   <si>
-    <t>Sonorant</t>
-  </si>
-  <si>
-    <t>Liquid</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>Stops</t>
-  </si>
-  <si>
-    <t>Affric</t>
-  </si>
-  <si>
-    <t>Fricat all</t>
-  </si>
-  <si>
-    <t>Sibil</t>
-  </si>
-  <si>
-    <t>Non-sibil</t>
-  </si>
-  <si>
-    <t>Approx</t>
-  </si>
-  <si>
-    <t>Trill</t>
-  </si>
-  <si>
-    <t>Flap</t>
-  </si>
-  <si>
-    <t>Lateral</t>
-  </si>
-  <si>
     <t>stone</t>
   </si>
   <si>
@@ -258,6 +222,32 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">�% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.0"/>
+        <rFont val="Calibri"/>
+        <vertAlign val="superscript"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">∞% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.0"/>
+        <rFont val="Calibri"/>
+        <vertAlign val="superscript"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">14,3% </t>
     </r>
     <r>
@@ -362,6 +352,32 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">0% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.0"/>
+        <rFont val="Calibri"/>
+        <vertAlign val="superscript"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">28,6% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.0"/>
+        <rFont val="Calibri"/>
+        <vertAlign val="superscript"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">0 </t>
     </r>
     <r>
@@ -491,6 +507,32 @@
     </r>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">� </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.0"/>
+        <rFont val="Calibri"/>
+        <vertAlign val="superscript"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">∞ </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.0"/>
+        <rFont val="Calibri"/>
+        <vertAlign val="superscript"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
     <t>leaf</t>
   </si>
   <si>
@@ -729,6 +771,19 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">18,2% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.0"/>
+        <rFont val="Calibri"/>
+        <vertAlign val="superscript"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">0,2 </t>
     </r>
     <r>
@@ -979,6 +1034,19 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">21,1% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.0"/>
+        <rFont val="Calibri"/>
+        <vertAlign val="superscript"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">0 </t>
     </r>
     <r>
@@ -1164,6 +1232,19 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">20,9% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.0"/>
+        <rFont val="Calibri"/>
+        <vertAlign val="superscript"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">0,3 </t>
     </r>
     <r>
@@ -1362,6 +1443,19 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">10% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.0"/>
+        <rFont val="Calibri"/>
+        <vertAlign val="superscript"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">1,5 </t>
     </r>
     <r>
@@ -1469,6 +1563,19 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">24,6% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.0"/>
+        <rFont val="Calibri"/>
+        <vertAlign val="superscript"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">0,4 </t>
     </r>
     <r>
@@ -1562,6 +1669,19 @@
     </r>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">14,1% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.0"/>
+        <rFont val="Calibri"/>
+        <vertAlign val="superscript"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
     <t>sand</t>
   </si>
   <si>
@@ -1670,6 +1790,19 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">14,5% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.0"/>
+        <rFont val="Calibri"/>
+        <vertAlign val="superscript"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">1,3 </t>
     </r>
     <r>
@@ -1724,6 +1857,19 @@
     </r>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">12,7% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.0"/>
+        <rFont val="Calibri"/>
+        <vertAlign val="superscript"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
     <t>nose</t>
   </si>
   <si>
@@ -1819,6 +1965,19 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">12,9% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.0"/>
+        <rFont val="Calibri"/>
+        <vertAlign val="superscript"/>
+      </rPr>
+      <t>0</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <t xml:space="preserve">0,8 </t>
     </r>
     <r>
@@ -2003,6 +2162,19 @@
         <vertAlign val="superscript"/>
       </rPr>
       <t>14</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">26,9% </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11.0"/>
+        <rFont val="Calibri"/>
+        <vertAlign val="superscript"/>
+      </rPr>
+      <t>0</t>
     </r>
   </si>
 </sst>
@@ -2011,13 +2183,373 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="433">
+  <fonts count="505">
     <font>
       <sz val="11.0"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <sz val="11.0"/>
+      <vertAlign val="superscript"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -4776,7 +5308,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AA15"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -4815,16 +5347,6 @@
         <v>22</v>
       </c>
       <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="1"/>
@@ -4854,20 +5376,6 @@
         <v>23</v>
       </c>
       <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1"/>
@@ -4909,356 +5417,364 @@
       <c r="O3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="2">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B4" t="n" s="3">
         <v>14.0</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" t="s" s="5">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E4" t="s" s="6">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s" s="7">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="G4" t="s" s="8">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="H4" t="s" s="9">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="I4" t="s" s="10">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="J4" t="s" s="11">
-        <v>41</v>
+        <v>29</v>
       </c>
       <c r="K4" t="s" s="12">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="L4" t="s" s="13">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="M4" t="s" s="14">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="N4" t="s" s="15">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="O4" t="s" s="16">
-        <v>46</v>
+        <v>34</v>
+      </c>
+      <c r="P4" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="17">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B5" t="n" s="18">
         <v>14.0</v>
       </c>
       <c r="C5" s="19"/>
       <c r="D5" t="s" s="20">
+        <v>61</v>
+      </c>
+      <c r="E5" t="s" s="21">
+        <v>60</v>
+      </c>
+      <c r="F5" t="s" s="22">
+        <v>63</v>
+      </c>
+      <c r="G5" t="s" s="23">
+        <v>64</v>
+      </c>
+      <c r="H5" t="s" s="24">
+        <v>32</v>
+      </c>
+      <c r="I5" t="s" s="25">
+        <v>62</v>
+      </c>
+      <c r="J5" t="s" s="26">
+        <v>29</v>
+      </c>
+      <c r="K5" t="s" s="27">
         <v>67</v>
       </c>
-      <c r="E5" t="s" s="21">
+      <c r="L5" t="s" s="28">
+        <v>65</v>
+      </c>
+      <c r="M5" t="s" s="29">
         <v>66</v>
       </c>
-      <c r="F5" t="s" s="22">
-        <v>69</v>
-      </c>
-      <c r="G5" t="s" s="23">
-        <v>70</v>
-      </c>
-      <c r="H5" t="s" s="24">
-        <v>44</v>
-      </c>
-      <c r="I5" t="s" s="25">
-        <v>68</v>
-      </c>
-      <c r="J5" t="s" s="26">
-        <v>41</v>
-      </c>
-      <c r="K5" t="s" s="27">
-        <v>73</v>
-      </c>
-      <c r="L5" t="s" s="28">
-        <v>71</v>
-      </c>
-      <c r="M5" t="s" s="29">
-        <v>72</v>
-      </c>
       <c r="N5" t="s" s="30">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="O5" t="s" s="31">
-        <v>46</v>
+        <v>34</v>
+      </c>
+      <c r="P5" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="32">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B6" t="n" s="33">
         <v>14.0</v>
       </c>
       <c r="C6" s="34"/>
       <c r="D6" t="s" s="35">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E6" t="s" s="36">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F6" t="s" s="37">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G6" t="s" s="38">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H6" t="s" s="39">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="I6" t="s" s="40">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="J6" t="s" s="41">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="K6" t="s" s="42">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="L6" t="s" s="43">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="M6" t="s" s="44">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="N6" t="s" s="45">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="O6" t="s" s="46">
-        <v>46</v>
+        <v>34</v>
+      </c>
+      <c r="P6" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="47">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B7" t="n" s="48">
         <v>13.0</v>
       </c>
       <c r="C7" s="49"/>
       <c r="D7" t="s" s="50">
+        <v>103</v>
+      </c>
+      <c r="E7" t="s" s="51">
+        <v>102</v>
+      </c>
+      <c r="F7" t="s" s="52">
+        <v>30</v>
+      </c>
+      <c r="G7" t="s" s="53">
+        <v>105</v>
+      </c>
+      <c r="H7" t="s" s="54">
+        <v>103</v>
+      </c>
+      <c r="I7" t="s" s="55">
+        <v>104</v>
+      </c>
+      <c r="J7" t="s" s="56">
+        <v>60</v>
+      </c>
+      <c r="K7" t="s" s="57">
+        <v>103</v>
+      </c>
+      <c r="L7" t="s" s="58">
+        <v>103</v>
+      </c>
+      <c r="M7" t="s" s="59">
+        <v>106</v>
+      </c>
+      <c r="N7" t="s" s="60">
+        <v>26</v>
+      </c>
+      <c r="O7" t="s" s="61">
         <v>107</v>
       </c>
-      <c r="E7" t="s" s="51">
-        <v>106</v>
-      </c>
-      <c r="F7" t="s" s="52">
-        <v>42</v>
-      </c>
-      <c r="G7" t="s" s="53">
-        <v>109</v>
-      </c>
-      <c r="H7" t="s" s="54">
-        <v>107</v>
-      </c>
-      <c r="I7" t="s" s="55">
-        <v>108</v>
-      </c>
-      <c r="J7" t="s" s="56">
-        <v>66</v>
-      </c>
-      <c r="K7" t="s" s="57">
-        <v>107</v>
-      </c>
-      <c r="L7" t="s" s="58">
-        <v>107</v>
-      </c>
-      <c r="M7" t="s" s="59">
-        <v>110</v>
-      </c>
-      <c r="N7" t="s" s="60">
-        <v>38</v>
-      </c>
-      <c r="O7" t="s" s="61">
-        <v>111</v>
+      <c r="P7" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="62">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B8" t="n" s="63">
         <v>14.0</v>
       </c>
       <c r="C8" s="64"/>
       <c r="D8" t="s" s="65">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="E8" t="s" s="66">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F8" t="s" s="67">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="G8" t="s" s="68">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H8" t="s" s="69">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="I8" t="s" s="70">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="J8" t="s" s="71">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="K8" t="s" s="72">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="L8" t="s" s="73">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="M8" t="s" s="74">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="N8" t="s" s="75">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="O8" t="s" s="76">
-        <v>46</v>
+        <v>34</v>
+      </c>
+      <c r="P8" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="77">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B9" t="n" s="78">
         <v>14.0</v>
       </c>
       <c r="C9" s="79"/>
       <c r="D9" t="s" s="80">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E9" t="s" s="81">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F9" t="s" s="82">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="G9" t="s" s="83">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="H9" t="s" s="84">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="I9" t="s" s="85">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="J9" t="s" s="86">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="K9" t="s" s="87">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="L9" t="s" s="88">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="M9" t="s" s="89">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="N9" t="s" s="90">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="O9" t="s" s="91">
-        <v>46</v>
+        <v>34</v>
+      </c>
+      <c r="P9" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="92">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B10" t="n" s="93">
         <v>14.0</v>
       </c>
       <c r="C10" s="94"/>
       <c r="D10" t="s" s="95">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="E10" t="s" s="96">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s" s="97">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="G10" t="s" s="98">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="H10" t="s" s="99">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I10" t="s" s="100">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="J10" t="s" s="101">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="K10" t="s" s="102">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="L10" t="s" s="103">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="M10" t="s" s="104">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="N10" t="s" s="105">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="O10" t="s" s="106">
-        <v>46</v>
+        <v>34</v>
+      </c>
+      <c r="P10" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="11">
@@ -5270,220 +5786,250 @@
       </c>
       <c r="C11" s="109"/>
       <c r="D11" t="s" s="110">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E11" t="s" s="111">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F11" t="s" s="112">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G11" t="s" s="113">
         <v>153</v>
       </c>
       <c r="H11" t="s" s="114">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="I11" t="s" s="115">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="J11" t="s" s="116">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="K11" t="s" s="117">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="L11" t="s" s="118">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="M11" t="s" s="119">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="N11" t="s" s="120">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="O11" t="s" s="121">
-        <v>46</v>
+        <v>34</v>
+      </c>
+      <c r="P11" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="122">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B12" t="n" s="123">
         <v>14.0</v>
       </c>
       <c r="C12" s="124"/>
       <c r="D12" t="s" s="125">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="E12" t="s" s="126">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="F12" t="s" s="127">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="G12" t="s" s="128">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="H12" t="s" s="129">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="I12" t="s" s="130">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="J12" t="s" s="131">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="K12" t="s" s="132">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="L12" t="s" s="133">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="M12" t="s" s="134">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="N12" t="s" s="135">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="O12" t="s" s="136">
-        <v>46</v>
+        <v>34</v>
+      </c>
+      <c r="P12" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="137">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B13" t="n" s="138">
         <v>14.0</v>
       </c>
       <c r="C13" s="139"/>
       <c r="D13" t="s" s="140">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E13" t="s" s="141">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F13" t="s" s="142">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="G13" t="s" s="143">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="H13" t="s" s="144">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="I13" t="s" s="145">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J13" t="s" s="146">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="K13" t="s" s="147">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="L13" t="s" s="148">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="M13" t="s" s="149">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="N13" t="s" s="150">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="O13" t="s" s="151">
-        <v>46</v>
+        <v>34</v>
+      </c>
+      <c r="P13" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="152">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B14" t="n" s="153">
         <v>14.0</v>
       </c>
       <c r="C14" s="154"/>
       <c r="D14" t="s" s="155">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E14" t="s" s="156">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F14" t="s" s="157">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="G14" t="s" s="158">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H14" t="s" s="159">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="I14" t="s" s="160">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="J14" t="s" s="161">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="K14" t="s" s="162">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="L14" t="s" s="163">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="M14" t="s" s="164">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="N14" t="s" s="165">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="O14" t="s" s="166">
-        <v>46</v>
+        <v>34</v>
+      </c>
+      <c r="P14" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="167">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B15" t="n" s="168">
         <v>14.0</v>
       </c>
       <c r="C15" s="169"/>
       <c r="D15" t="s" s="170">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="E15" t="s" s="171">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F15" t="s" s="172">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="G15" t="s" s="173">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="H15" t="s" s="174">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="I15" t="s" s="175">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="J15" t="s" s="176">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="K15" t="s" s="177">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="L15" t="s" s="178">
-        <v>40</v>
+        <v>28</v>
       </c>
       <c r="M15" t="s" s="179">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="N15" t="s" s="180">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="O15" t="s" s="181">
-        <v>46</v>
+        <v>34</v>
+      </c>
+      <c r="P15" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -5496,7 +6042,7 @@
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P1:AA1"/>
+    <mergeCell ref="P1:R1"/>
     <mergeCell ref="P2:U2"/>
     <mergeCell ref="V2:Z2"/>
   </mergeCells>
@@ -5506,7 +6052,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AA15"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -5545,16 +6091,6 @@
         <v>22</v>
       </c>
       <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="1"/>
@@ -5584,20 +6120,6 @@
         <v>23</v>
       </c>
       <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1"/>
@@ -5639,356 +6161,364 @@
       <c r="O3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="182">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B4" t="n" s="183">
         <v>14.0</v>
       </c>
       <c r="C4" s="184"/>
       <c r="D4" t="s" s="185">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="E4" t="s" s="186">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F4" t="s" s="187">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G4" t="s" s="188">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="H4" t="s" s="189">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="I4" t="s" s="190">
-        <v>48</v>
+        <v>38</v>
       </c>
       <c r="J4" t="s" s="191">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="K4" t="s" s="192">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="L4" t="s" s="193">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="M4" t="s" s="194">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="N4" t="s" s="195">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="O4" t="s" s="196">
+        <v>34</v>
+      </c>
+      <c r="P4" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q4" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="197">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B5" t="n" s="198">
         <v>14.0</v>
       </c>
       <c r="C5" s="199"/>
       <c r="D5" t="s" s="200">
+        <v>69</v>
+      </c>
+      <c r="E5" t="s" s="201">
+        <v>68</v>
+      </c>
+      <c r="F5" t="s" s="202">
+        <v>72</v>
+      </c>
+      <c r="G5" t="s" s="203">
+        <v>73</v>
+      </c>
+      <c r="H5" t="s" s="204">
+        <v>77</v>
+      </c>
+      <c r="I5" t="s" s="205">
+        <v>70</v>
+      </c>
+      <c r="J5" t="s" s="206">
+        <v>71</v>
+      </c>
+      <c r="K5" t="s" s="207">
+        <v>76</v>
+      </c>
+      <c r="L5" t="s" s="208">
+        <v>74</v>
+      </c>
+      <c r="M5" t="s" s="209">
         <v>75</v>
       </c>
-      <c r="E5" t="s" s="201">
-        <v>74</v>
-      </c>
-      <c r="F5" t="s" s="202">
+      <c r="N5" t="s" s="210">
+        <v>26</v>
+      </c>
+      <c r="O5" t="s" s="211">
+        <v>34</v>
+      </c>
+      <c r="P5" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q5" t="s">
         <v>78</v>
-      </c>
-      <c r="G5" t="s" s="203">
-        <v>79</v>
-      </c>
-      <c r="H5" t="s" s="204">
-        <v>83</v>
-      </c>
-      <c r="I5" t="s" s="205">
-        <v>76</v>
-      </c>
-      <c r="J5" t="s" s="206">
-        <v>77</v>
-      </c>
-      <c r="K5" t="s" s="207">
-        <v>82</v>
-      </c>
-      <c r="L5" t="s" s="208">
-        <v>80</v>
-      </c>
-      <c r="M5" t="s" s="209">
-        <v>81</v>
-      </c>
-      <c r="N5" t="s" s="210">
-        <v>38</v>
-      </c>
-      <c r="O5" t="s" s="211">
-        <v>46</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="212">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B6" t="n" s="213">
         <v>14.0</v>
       </c>
       <c r="C6" s="214"/>
       <c r="D6" t="s" s="215">
+        <v>93</v>
+      </c>
+      <c r="E6" t="s" s="216">
+        <v>92</v>
+      </c>
+      <c r="F6" t="s" s="217">
+        <v>90</v>
+      </c>
+      <c r="G6" t="s" s="218">
+        <v>95</v>
+      </c>
+      <c r="H6" t="s" s="219">
         <v>98</v>
       </c>
-      <c r="E6" t="s" s="216">
+      <c r="I6" t="s" s="220">
+        <v>94</v>
+      </c>
+      <c r="J6" t="s" s="221">
+        <v>25</v>
+      </c>
+      <c r="K6" t="s" s="222">
+        <v>93</v>
+      </c>
+      <c r="L6" t="s" s="223">
+        <v>96</v>
+      </c>
+      <c r="M6" t="s" s="224">
         <v>97</v>
       </c>
-      <c r="F6" t="s" s="217">
-        <v>95</v>
-      </c>
-      <c r="G6" t="s" s="218">
-        <v>100</v>
-      </c>
-      <c r="H6" t="s" s="219">
-        <v>103</v>
-      </c>
-      <c r="I6" t="s" s="220">
+      <c r="N6" t="s" s="225">
+        <v>26</v>
+      </c>
+      <c r="O6" t="s" s="226">
+        <v>34</v>
+      </c>
+      <c r="P6" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q6" t="s">
         <v>99</v>
-      </c>
-      <c r="J6" t="s" s="221">
-        <v>37</v>
-      </c>
-      <c r="K6" t="s" s="222">
-        <v>98</v>
-      </c>
-      <c r="L6" t="s" s="223">
-        <v>101</v>
-      </c>
-      <c r="M6" t="s" s="224">
-        <v>102</v>
-      </c>
-      <c r="N6" t="s" s="225">
-        <v>38</v>
-      </c>
-      <c r="O6" t="s" s="226">
-        <v>46</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="227">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B7" t="n" s="228">
         <v>13.0</v>
       </c>
       <c r="C7" s="229"/>
       <c r="D7" t="s" s="230">
+        <v>109</v>
+      </c>
+      <c r="E7" t="s" s="231">
+        <v>108</v>
+      </c>
+      <c r="F7" t="s" s="232">
+        <v>111</v>
+      </c>
+      <c r="G7" t="s" s="233">
+        <v>112</v>
+      </c>
+      <c r="H7" t="s" s="234">
+        <v>114</v>
+      </c>
+      <c r="I7" t="s" s="235">
+        <v>110</v>
+      </c>
+      <c r="J7" t="s" s="236">
+        <v>68</v>
+      </c>
+      <c r="K7" t="s" s="237">
         <v>113</v>
       </c>
-      <c r="E7" t="s" s="231">
-        <v>112</v>
-      </c>
-      <c r="F7" t="s" s="232">
+      <c r="L7" t="s" s="238">
+        <v>109</v>
+      </c>
+      <c r="M7" t="s" s="239">
+        <v>110</v>
+      </c>
+      <c r="N7" t="s" s="240">
+        <v>26</v>
+      </c>
+      <c r="O7" t="s" s="241">
+        <v>107</v>
+      </c>
+      <c r="P7" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q7" t="s">
         <v>115</v>
-      </c>
-      <c r="G7" t="s" s="233">
-        <v>116</v>
-      </c>
-      <c r="H7" t="s" s="234">
-        <v>118</v>
-      </c>
-      <c r="I7" t="s" s="235">
-        <v>114</v>
-      </c>
-      <c r="J7" t="s" s="236">
-        <v>74</v>
-      </c>
-      <c r="K7" t="s" s="237">
-        <v>117</v>
-      </c>
-      <c r="L7" t="s" s="238">
-        <v>113</v>
-      </c>
-      <c r="M7" t="s" s="239">
-        <v>114</v>
-      </c>
-      <c r="N7" t="s" s="240">
-        <v>38</v>
-      </c>
-      <c r="O7" t="s" s="241">
-        <v>111</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="242">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B8" t="n" s="243">
         <v>14.0</v>
       </c>
       <c r="C8" s="244"/>
       <c r="D8" t="s" s="245">
+        <v>124</v>
+      </c>
+      <c r="E8" t="s" s="246">
+        <v>25</v>
+      </c>
+      <c r="F8" t="s" s="247">
         <v>127</v>
       </c>
-      <c r="E8" t="s" s="246">
-        <v>37</v>
-      </c>
-      <c r="F8" t="s" s="247">
+      <c r="G8" t="s" s="248">
+        <v>128</v>
+      </c>
+      <c r="H8" t="s" s="249">
+        <v>131</v>
+      </c>
+      <c r="I8" t="s" s="250">
+        <v>125</v>
+      </c>
+      <c r="J8" t="s" s="251">
+        <v>126</v>
+      </c>
+      <c r="K8" t="s" s="252">
         <v>130</v>
       </c>
-      <c r="G8" t="s" s="248">
-        <v>131</v>
-      </c>
-      <c r="H8" t="s" s="249">
-        <v>134</v>
-      </c>
-      <c r="I8" t="s" s="250">
-        <v>128</v>
-      </c>
-      <c r="J8" t="s" s="251">
+      <c r="L8" t="s" s="253">
+        <v>98</v>
+      </c>
+      <c r="M8" t="s" s="254">
         <v>129</v>
       </c>
-      <c r="K8" t="s" s="252">
-        <v>133</v>
-      </c>
-      <c r="L8" t="s" s="253">
-        <v>103</v>
-      </c>
-      <c r="M8" t="s" s="254">
+      <c r="N8" t="s" s="255">
+        <v>26</v>
+      </c>
+      <c r="O8" t="s" s="256">
+        <v>34</v>
+      </c>
+      <c r="P8" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q8" t="s">
         <v>132</v>
-      </c>
-      <c r="N8" t="s" s="255">
-        <v>38</v>
-      </c>
-      <c r="O8" t="s" s="256">
-        <v>46</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="257">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B9" t="n" s="258">
         <v>14.0</v>
       </c>
       <c r="C9" s="259"/>
       <c r="D9" t="s" s="260">
+        <v>136</v>
+      </c>
+      <c r="E9" t="s" s="261">
+        <v>68</v>
+      </c>
+      <c r="F9" t="s" s="262">
+        <v>111</v>
+      </c>
+      <c r="G9" t="s" s="263">
         <v>138</v>
       </c>
-      <c r="E9" t="s" s="261">
-        <v>74</v>
-      </c>
-      <c r="F9" t="s" s="262">
-        <v>115</v>
-      </c>
-      <c r="G9" t="s" s="263">
+      <c r="H9" t="s" s="264">
+        <v>141</v>
+      </c>
+      <c r="I9" t="s" s="265">
+        <v>137</v>
+      </c>
+      <c r="J9" t="s" s="266">
+        <v>68</v>
+      </c>
+      <c r="K9" t="s" s="267">
         <v>140</v>
       </c>
-      <c r="H9" t="s" s="264">
-        <v>143</v>
-      </c>
-      <c r="I9" t="s" s="265">
+      <c r="L9" t="s" s="268">
         <v>139</v>
       </c>
-      <c r="J9" t="s" s="266">
-        <v>74</v>
-      </c>
-      <c r="K9" t="s" s="267">
+      <c r="M9" t="s" s="269">
+        <v>137</v>
+      </c>
+      <c r="N9" t="s" s="270">
+        <v>26</v>
+      </c>
+      <c r="O9" t="s" s="271">
+        <v>34</v>
+      </c>
+      <c r="P9" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q9" t="s">
         <v>142</v>
-      </c>
-      <c r="L9" t="s" s="268">
-        <v>141</v>
-      </c>
-      <c r="M9" t="s" s="269">
-        <v>139</v>
-      </c>
-      <c r="N9" t="s" s="270">
-        <v>38</v>
-      </c>
-      <c r="O9" t="s" s="271">
-        <v>46</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="272">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B10" t="n" s="273">
         <v>14.0</v>
       </c>
       <c r="C10" s="274"/>
       <c r="D10" t="s" s="275">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="E10" t="s" s="276">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F10" t="s" s="277">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G10" t="s" s="278">
+        <v>149</v>
+      </c>
+      <c r="H10" t="s" s="279">
+        <v>124</v>
+      </c>
+      <c r="I10" t="s" s="280">
+        <v>147</v>
+      </c>
+      <c r="J10" t="s" s="281">
+        <v>148</v>
+      </c>
+      <c r="K10" t="s" s="282">
         <v>150</v>
       </c>
-      <c r="H10" t="s" s="279">
-        <v>127</v>
-      </c>
-      <c r="I10" t="s" s="280">
-        <v>148</v>
-      </c>
-      <c r="J10" t="s" s="281">
-        <v>149</v>
-      </c>
-      <c r="K10" t="s" s="282">
+      <c r="L10" t="s" s="283">
+        <v>131</v>
+      </c>
+      <c r="M10" t="s" s="284">
+        <v>147</v>
+      </c>
+      <c r="N10" t="s" s="285">
+        <v>26</v>
+      </c>
+      <c r="O10" t="s" s="286">
+        <v>34</v>
+      </c>
+      <c r="P10" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q10" t="s">
         <v>151</v>
-      </c>
-      <c r="L10" t="s" s="283">
-        <v>134</v>
-      </c>
-      <c r="M10" t="s" s="284">
-        <v>148</v>
-      </c>
-      <c r="N10" t="s" s="285">
-        <v>38</v>
-      </c>
-      <c r="O10" t="s" s="286">
-        <v>46</v>
       </c>
     </row>
     <row r="11">
@@ -6000,13 +6530,13 @@
       </c>
       <c r="C11" s="289"/>
       <c r="D11" t="s" s="290">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E11" t="s" s="291">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F11" t="s" s="292">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="G11" t="s" s="293">
         <v>156</v>
@@ -6030,130 +6560,148 @@
         <v>158</v>
       </c>
       <c r="N11" t="s" s="300">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="O11" t="s" s="301">
-        <v>46</v>
+        <v>34</v>
+      </c>
+      <c r="P11" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="302">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B12" t="n" s="303">
         <v>14.0</v>
       </c>
       <c r="C12" s="304"/>
       <c r="D12" t="s" s="305">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s" s="306">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F12" t="s" s="307">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G12" t="s" s="308">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="H12" t="s" s="309">
+        <v>166</v>
+      </c>
+      <c r="I12" t="s" s="310">
         <v>165</v>
       </c>
-      <c r="I12" t="s" s="310">
-        <v>164</v>
-      </c>
       <c r="J12" t="s" s="311">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="K12" t="s" s="312">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="L12" t="s" s="313">
-        <v>47</v>
+        <v>37</v>
       </c>
       <c r="M12" t="s" s="314">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="N12" t="s" s="315">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="O12" t="s" s="316">
-        <v>46</v>
+        <v>34</v>
+      </c>
+      <c r="P12" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="317">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B13" t="n" s="318">
         <v>14.0</v>
       </c>
       <c r="C13" s="319"/>
       <c r="D13" t="s" s="320">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="E13" t="s" s="321">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="F13" t="s" s="322">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="G13" t="s" s="323">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="H13" t="s" s="324">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="I13" t="s" s="325">
+        <v>171</v>
+      </c>
+      <c r="J13" t="s" s="326">
         <v>169</v>
       </c>
-      <c r="J13" t="s" s="326">
-        <v>167</v>
-      </c>
       <c r="K13" t="s" s="327">
+        <v>175</v>
+      </c>
+      <c r="L13" t="s" s="328">
         <v>173</v>
       </c>
-      <c r="L13" t="s" s="328">
-        <v>171</v>
-      </c>
       <c r="M13" t="s" s="329">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="N13" t="s" s="330">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="O13" t="s" s="331">
-        <v>46</v>
+        <v>34</v>
+      </c>
+      <c r="P13" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="332">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B14" t="n" s="333">
         <v>14.0</v>
       </c>
       <c r="C14" s="334"/>
       <c r="D14" t="s" s="335">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="E14" t="s" s="336">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F14" t="s" s="337">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="G14" t="s" s="338">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="H14" t="s" s="339">
         <v>159</v>
       </c>
       <c r="I14" t="s" s="340">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="J14" t="s" s="341">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="K14" t="s" s="342">
         <v>159</v>
@@ -6162,58 +6710,70 @@
         <v>159</v>
       </c>
       <c r="M14" t="s" s="344">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="N14" t="s" s="345">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="O14" t="s" s="346">
-        <v>46</v>
+        <v>34</v>
+      </c>
+      <c r="P14" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="347">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B15" t="n" s="348">
         <v>14.0</v>
       </c>
       <c r="C15" s="349"/>
       <c r="D15" t="s" s="350">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E15" t="s" s="351">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F15" t="s" s="352">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="G15" t="s" s="353">
+        <v>190</v>
+      </c>
+      <c r="H15" t="s" s="354">
+        <v>192</v>
+      </c>
+      <c r="I15" t="s" s="355">
         <v>187</v>
       </c>
-      <c r="H15" t="s" s="354">
-        <v>189</v>
-      </c>
-      <c r="I15" t="s" s="355">
-        <v>184</v>
-      </c>
       <c r="J15" t="s" s="356">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="K15" t="s" s="357">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="L15" t="s" s="358">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="M15" t="s" s="359">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="N15" t="s" s="360">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="O15" t="s" s="361">
-        <v>46</v>
+        <v>34</v>
+      </c>
+      <c r="P15" t="s">
+        <v>45</v>
+      </c>
+      <c r="Q15" t="s">
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -6226,7 +6786,7 @@
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P1:AA1"/>
+    <mergeCell ref="P1:R1"/>
     <mergeCell ref="P2:U2"/>
     <mergeCell ref="V2:Z2"/>
   </mergeCells>
@@ -6236,7 +6796,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:AA15"/>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -6275,16 +6835,6 @@
         <v>22</v>
       </c>
       <c r="Q1" s="1"/>
-      <c r="R1" s="1"/>
-      <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
-      <c r="V1" s="1"/>
-      <c r="W1" s="1"/>
-      <c r="X1" s="1"/>
-      <c r="Y1" s="1"/>
-      <c r="Z1" s="1"/>
-      <c r="AA1" s="1"/>
     </row>
     <row r="2">
       <c r="A2" s="1"/>
@@ -6314,20 +6864,6 @@
         <v>23</v>
       </c>
       <c r="Q2" s="1"/>
-      <c r="R2" s="1"/>
-      <c r="S2" s="1"/>
-      <c r="T2" s="1"/>
-      <c r="U2" s="1"/>
-      <c r="V2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="W2" s="1"/>
-      <c r="X2" s="1"/>
-      <c r="Y2" s="1"/>
-      <c r="Z2" s="1"/>
-      <c r="AA2" s="1" t="s">
-        <v>25</v>
-      </c>
     </row>
     <row r="3">
       <c r="A3" s="1"/>
@@ -6369,356 +6905,364 @@
       <c r="O3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="P3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="S3" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="W3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="X3" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="Y3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="Z3" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA3" s="1" t="s">
-        <v>35</v>
-      </c>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
     </row>
     <row r="4">
       <c r="A4" t="s" s="362">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="B4" t="n" s="363">
         <v>14.0</v>
       </c>
       <c r="C4" s="364"/>
       <c r="D4" t="s" s="365">
+        <v>49</v>
+      </c>
+      <c r="E4" t="s" s="366">
+        <v>47</v>
+      </c>
+      <c r="F4" t="s" s="367">
+        <v>52</v>
+      </c>
+      <c r="G4" t="s" s="368">
+        <v>53</v>
+      </c>
+      <c r="H4" t="s" s="369">
+        <v>56</v>
+      </c>
+      <c r="I4" t="s" s="370">
+        <v>50</v>
+      </c>
+      <c r="J4" t="s" s="371">
+        <v>51</v>
+      </c>
+      <c r="K4" t="s" s="372">
+        <v>49</v>
+      </c>
+      <c r="L4" t="s" s="373">
+        <v>49</v>
+      </c>
+      <c r="M4" t="s" s="374">
+        <v>54</v>
+      </c>
+      <c r="N4" t="s" s="375">
+        <v>48</v>
+      </c>
+      <c r="O4" t="s" s="376">
+        <v>55</v>
+      </c>
+      <c r="P4" t="s">
         <v>57</v>
       </c>
-      <c r="E4" t="s" s="366">
-        <v>55</v>
-      </c>
-      <c r="F4" t="s" s="367">
-        <v>60</v>
-      </c>
-      <c r="G4" t="s" s="368">
-        <v>61</v>
-      </c>
-      <c r="H4" t="s" s="369">
-        <v>64</v>
-      </c>
-      <c r="I4" t="s" s="370">
+      <c r="Q4" t="s">
         <v>58</v>
-      </c>
-      <c r="J4" t="s" s="371">
-        <v>59</v>
-      </c>
-      <c r="K4" t="s" s="372">
-        <v>57</v>
-      </c>
-      <c r="L4" t="s" s="373">
-        <v>57</v>
-      </c>
-      <c r="M4" t="s" s="374">
-        <v>62</v>
-      </c>
-      <c r="N4" t="s" s="375">
-        <v>56</v>
-      </c>
-      <c r="O4" t="s" s="376">
-        <v>63</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="377">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="B5" t="n" s="378">
         <v>14.0</v>
       </c>
       <c r="C5" s="379"/>
       <c r="D5" t="s" s="380">
+        <v>49</v>
+      </c>
+      <c r="E5" t="s" s="381">
+        <v>79</v>
+      </c>
+      <c r="F5" t="s" s="382">
+        <v>82</v>
+      </c>
+      <c r="G5" t="s" s="383">
+        <v>83</v>
+      </c>
+      <c r="H5" t="s" s="384">
+        <v>87</v>
+      </c>
+      <c r="I5" t="s" s="385">
+        <v>80</v>
+      </c>
+      <c r="J5" t="s" s="386">
+        <v>81</v>
+      </c>
+      <c r="K5" t="s" s="387">
+        <v>86</v>
+      </c>
+      <c r="L5" t="s" s="388">
+        <v>84</v>
+      </c>
+      <c r="M5" t="s" s="389">
+        <v>85</v>
+      </c>
+      <c r="N5" t="s" s="390">
+        <v>48</v>
+      </c>
+      <c r="O5" t="s" s="391">
+        <v>55</v>
+      </c>
+      <c r="P5" t="s">
         <v>57</v>
       </c>
-      <c r="E5" t="s" s="381">
-        <v>84</v>
-      </c>
-      <c r="F5" t="s" s="382">
-        <v>87</v>
-      </c>
-      <c r="G5" t="s" s="383">
-        <v>88</v>
-      </c>
-      <c r="H5" t="s" s="384">
-        <v>92</v>
-      </c>
-      <c r="I5" t="s" s="385">
-        <v>85</v>
-      </c>
-      <c r="J5" t="s" s="386">
-        <v>86</v>
-      </c>
-      <c r="K5" t="s" s="387">
-        <v>91</v>
-      </c>
-      <c r="L5" t="s" s="388">
-        <v>89</v>
-      </c>
-      <c r="M5" t="s" s="389">
-        <v>90</v>
-      </c>
-      <c r="N5" t="s" s="390">
-        <v>56</v>
-      </c>
-      <c r="O5" t="s" s="391">
-        <v>63</v>
+      <c r="Q5" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="392">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B6" t="n" s="393">
         <v>14.0</v>
       </c>
       <c r="C6" s="394"/>
       <c r="D6" t="s" s="395">
+        <v>49</v>
+      </c>
+      <c r="E6" t="s" s="396">
+        <v>79</v>
+      </c>
+      <c r="F6" t="s" s="397">
+        <v>100</v>
+      </c>
+      <c r="G6" t="s" s="398">
+        <v>83</v>
+      </c>
+      <c r="H6" t="s" s="399">
+        <v>56</v>
+      </c>
+      <c r="I6" t="s" s="400">
+        <v>80</v>
+      </c>
+      <c r="J6" t="s" s="401">
+        <v>47</v>
+      </c>
+      <c r="K6" t="s" s="402">
+        <v>49</v>
+      </c>
+      <c r="L6" t="s" s="403">
+        <v>49</v>
+      </c>
+      <c r="M6" t="s" s="404">
+        <v>54</v>
+      </c>
+      <c r="N6" t="s" s="405">
+        <v>48</v>
+      </c>
+      <c r="O6" t="s" s="406">
+        <v>55</v>
+      </c>
+      <c r="P6" t="s">
         <v>57</v>
       </c>
-      <c r="E6" t="s" s="396">
-        <v>84</v>
-      </c>
-      <c r="F6" t="s" s="397">
-        <v>104</v>
-      </c>
-      <c r="G6" t="s" s="398">
-        <v>88</v>
-      </c>
-      <c r="H6" t="s" s="399">
-        <v>64</v>
-      </c>
-      <c r="I6" t="s" s="400">
-        <v>85</v>
-      </c>
-      <c r="J6" t="s" s="401">
-        <v>55</v>
-      </c>
-      <c r="K6" t="s" s="402">
-        <v>57</v>
-      </c>
-      <c r="L6" t="s" s="403">
-        <v>57</v>
-      </c>
-      <c r="M6" t="s" s="404">
-        <v>62</v>
-      </c>
-      <c r="N6" t="s" s="405">
-        <v>56</v>
-      </c>
-      <c r="O6" t="s" s="406">
-        <v>63</v>
+      <c r="Q6" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="407">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B7" t="n" s="408">
         <v>13.0</v>
       </c>
       <c r="C7" s="409"/>
       <c r="D7" t="s" s="410">
+        <v>117</v>
+      </c>
+      <c r="E7" t="s" s="411">
+        <v>116</v>
+      </c>
+      <c r="F7" t="s" s="412">
+        <v>52</v>
+      </c>
+      <c r="G7" t="s" s="413">
+        <v>119</v>
+      </c>
+      <c r="H7" t="s" s="414">
+        <v>122</v>
+      </c>
+      <c r="I7" t="s" s="415">
+        <v>118</v>
+      </c>
+      <c r="J7" t="s" s="416">
+        <v>79</v>
+      </c>
+      <c r="K7" t="s" s="417">
+        <v>121</v>
+      </c>
+      <c r="L7" t="s" s="418">
+        <v>117</v>
+      </c>
+      <c r="M7" t="s" s="419">
+        <v>118</v>
+      </c>
+      <c r="N7" t="s" s="420">
+        <v>48</v>
+      </c>
+      <c r="O7" t="s" s="421">
         <v>120</v>
       </c>
-      <c r="E7" t="s" s="411">
-        <v>119</v>
-      </c>
-      <c r="F7" t="s" s="412">
-        <v>60</v>
-      </c>
-      <c r="G7" t="s" s="413">
-        <v>122</v>
-      </c>
-      <c r="H7" t="s" s="414">
-        <v>125</v>
-      </c>
-      <c r="I7" t="s" s="415">
-        <v>121</v>
-      </c>
-      <c r="J7" t="s" s="416">
-        <v>84</v>
-      </c>
-      <c r="K7" t="s" s="417">
-        <v>124</v>
-      </c>
-      <c r="L7" t="s" s="418">
-        <v>120</v>
-      </c>
-      <c r="M7" t="s" s="419">
-        <v>121</v>
-      </c>
-      <c r="N7" t="s" s="420">
-        <v>56</v>
-      </c>
-      <c r="O7" t="s" s="421">
-        <v>123</v>
+      <c r="P7" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="422">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="B8" t="n" s="423">
         <v>14.0</v>
       </c>
       <c r="C8" s="424"/>
       <c r="D8" t="s" s="425">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="E8" t="s" s="426">
+        <v>47</v>
+      </c>
+      <c r="F8" t="s" s="427">
+        <v>52</v>
+      </c>
+      <c r="G8" t="s" s="428">
+        <v>121</v>
+      </c>
+      <c r="H8" t="s" s="429">
+        <v>56</v>
+      </c>
+      <c r="I8" t="s" s="430">
+        <v>133</v>
+      </c>
+      <c r="J8" t="s" s="431">
+        <v>79</v>
+      </c>
+      <c r="K8" t="s" s="432">
+        <v>50</v>
+      </c>
+      <c r="L8" t="s" s="433">
+        <v>134</v>
+      </c>
+      <c r="M8" t="s" s="434">
+        <v>85</v>
+      </c>
+      <c r="N8" t="s" s="435">
+        <v>48</v>
+      </c>
+      <c r="O8" t="s" s="436">
         <v>55</v>
       </c>
-      <c r="F8" t="s" s="427">
-        <v>60</v>
-      </c>
-      <c r="G8" t="s" s="428">
-        <v>124</v>
-      </c>
-      <c r="H8" t="s" s="429">
-        <v>64</v>
-      </c>
-      <c r="I8" t="s" s="430">
-        <v>135</v>
-      </c>
-      <c r="J8" t="s" s="431">
-        <v>84</v>
-      </c>
-      <c r="K8" t="s" s="432">
+      <c r="P8" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q8" t="s">
         <v>58</v>
-      </c>
-      <c r="L8" t="s" s="433">
-        <v>136</v>
-      </c>
-      <c r="M8" t="s" s="434">
-        <v>90</v>
-      </c>
-      <c r="N8" t="s" s="435">
-        <v>56</v>
-      </c>
-      <c r="O8" t="s" s="436">
-        <v>63</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="437">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B9" t="n" s="438">
         <v>14.0</v>
       </c>
       <c r="C9" s="439"/>
       <c r="D9" t="s" s="440">
+        <v>49</v>
+      </c>
+      <c r="E9" t="s" s="441">
+        <v>79</v>
+      </c>
+      <c r="F9" t="s" s="442">
+        <v>52</v>
+      </c>
+      <c r="G9" t="s" s="443">
+        <v>143</v>
+      </c>
+      <c r="H9" t="s" s="444">
+        <v>50</v>
+      </c>
+      <c r="I9" t="s" s="445">
+        <v>133</v>
+      </c>
+      <c r="J9" t="s" s="446">
+        <v>79</v>
+      </c>
+      <c r="K9" t="s" s="447">
+        <v>87</v>
+      </c>
+      <c r="L9" t="s" s="448">
+        <v>144</v>
+      </c>
+      <c r="M9" t="s" s="449">
+        <v>133</v>
+      </c>
+      <c r="N9" t="s" s="450">
+        <v>48</v>
+      </c>
+      <c r="O9" t="s" s="451">
+        <v>55</v>
+      </c>
+      <c r="P9" t="s">
         <v>57</v>
       </c>
-      <c r="E9" t="s" s="441">
-        <v>84</v>
-      </c>
-      <c r="F9" t="s" s="442">
-        <v>60</v>
-      </c>
-      <c r="G9" t="s" s="443">
-        <v>144</v>
-      </c>
-      <c r="H9" t="s" s="444">
+      <c r="Q9" t="s">
         <v>58</v>
-      </c>
-      <c r="I9" t="s" s="445">
-        <v>135</v>
-      </c>
-      <c r="J9" t="s" s="446">
-        <v>84</v>
-      </c>
-      <c r="K9" t="s" s="447">
-        <v>92</v>
-      </c>
-      <c r="L9" t="s" s="448">
-        <v>145</v>
-      </c>
-      <c r="M9" t="s" s="449">
-        <v>135</v>
-      </c>
-      <c r="N9" t="s" s="450">
-        <v>56</v>
-      </c>
-      <c r="O9" t="s" s="451">
-        <v>63</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="452">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B10" t="n" s="453">
         <v>14.0</v>
       </c>
       <c r="C10" s="454"/>
       <c r="D10" t="s" s="455">
+        <v>50</v>
+      </c>
+      <c r="E10" t="s" s="456">
+        <v>47</v>
+      </c>
+      <c r="F10" t="s" s="457">
+        <v>52</v>
+      </c>
+      <c r="G10" t="s" s="458">
+        <v>53</v>
+      </c>
+      <c r="H10" t="s" s="459">
+        <v>50</v>
+      </c>
+      <c r="I10" t="s" s="460">
+        <v>85</v>
+      </c>
+      <c r="J10" t="s" s="461">
+        <v>79</v>
+      </c>
+      <c r="K10" t="s" s="462">
+        <v>144</v>
+      </c>
+      <c r="L10" t="s" s="463">
+        <v>49</v>
+      </c>
+      <c r="M10" t="s" s="464">
+        <v>85</v>
+      </c>
+      <c r="N10" t="s" s="465">
+        <v>48</v>
+      </c>
+      <c r="O10" t="s" s="466">
+        <v>55</v>
+      </c>
+      <c r="P10" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q10" t="s">
         <v>58</v>
-      </c>
-      <c r="E10" t="s" s="456">
-        <v>55</v>
-      </c>
-      <c r="F10" t="s" s="457">
-        <v>60</v>
-      </c>
-      <c r="G10" t="s" s="458">
-        <v>61</v>
-      </c>
-      <c r="H10" t="s" s="459">
-        <v>58</v>
-      </c>
-      <c r="I10" t="s" s="460">
-        <v>90</v>
-      </c>
-      <c r="J10" t="s" s="461">
-        <v>84</v>
-      </c>
-      <c r="K10" t="s" s="462">
-        <v>145</v>
-      </c>
-      <c r="L10" t="s" s="463">
-        <v>57</v>
-      </c>
-      <c r="M10" t="s" s="464">
-        <v>90</v>
-      </c>
-      <c r="N10" t="s" s="465">
-        <v>56</v>
-      </c>
-      <c r="O10" t="s" s="466">
-        <v>63</v>
       </c>
     </row>
     <row r="11">
@@ -6730,220 +7274,250 @@
       </c>
       <c r="C11" s="469"/>
       <c r="D11" t="s" s="470">
+        <v>49</v>
+      </c>
+      <c r="E11" t="s" s="471">
+        <v>79</v>
+      </c>
+      <c r="F11" t="s" s="472">
+        <v>100</v>
+      </c>
+      <c r="G11" t="s" s="473">
+        <v>143</v>
+      </c>
+      <c r="H11" t="s" s="474">
+        <v>54</v>
+      </c>
+      <c r="I11" t="s" s="475">
+        <v>80</v>
+      </c>
+      <c r="J11" t="s" s="476">
+        <v>116</v>
+      </c>
+      <c r="K11" t="s" s="477">
+        <v>50</v>
+      </c>
+      <c r="L11" t="s" s="478">
+        <v>50</v>
+      </c>
+      <c r="M11" t="s" s="479">
+        <v>162</v>
+      </c>
+      <c r="N11" t="s" s="480">
+        <v>48</v>
+      </c>
+      <c r="O11" t="s" s="481">
+        <v>55</v>
+      </c>
+      <c r="P11" t="s">
         <v>57</v>
       </c>
-      <c r="E11" t="s" s="471">
-        <v>84</v>
-      </c>
-      <c r="F11" t="s" s="472">
-        <v>104</v>
-      </c>
-      <c r="G11" t="s" s="473">
-        <v>144</v>
-      </c>
-      <c r="H11" t="s" s="474">
-        <v>62</v>
-      </c>
-      <c r="I11" t="s" s="475">
-        <v>85</v>
-      </c>
-      <c r="J11" t="s" s="476">
-        <v>119</v>
-      </c>
-      <c r="K11" t="s" s="477">
+      <c r="Q11" t="s">
         <v>58</v>
-      </c>
-      <c r="L11" t="s" s="478">
-        <v>58</v>
-      </c>
-      <c r="M11" t="s" s="479">
-        <v>161</v>
-      </c>
-      <c r="N11" t="s" s="480">
-        <v>56</v>
-      </c>
-      <c r="O11" t="s" s="481">
-        <v>63</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="482">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B12" t="n" s="483">
         <v>14.0</v>
       </c>
       <c r="C12" s="484"/>
       <c r="D12" t="s" s="485">
+        <v>49</v>
+      </c>
+      <c r="E12" t="s" s="486">
+        <v>79</v>
+      </c>
+      <c r="F12" t="s" s="487">
+        <v>52</v>
+      </c>
+      <c r="G12" t="s" s="488">
+        <v>53</v>
+      </c>
+      <c r="H12" t="s" s="489">
+        <v>50</v>
+      </c>
+      <c r="I12" t="s" s="490">
+        <v>80</v>
+      </c>
+      <c r="J12" t="s" s="491">
+        <v>79</v>
+      </c>
+      <c r="K12" t="s" s="492">
+        <v>49</v>
+      </c>
+      <c r="L12" t="s" s="493">
+        <v>49</v>
+      </c>
+      <c r="M12" t="s" s="494">
+        <v>80</v>
+      </c>
+      <c r="N12" t="s" s="495">
+        <v>48</v>
+      </c>
+      <c r="O12" t="s" s="496">
+        <v>55</v>
+      </c>
+      <c r="P12" t="s">
         <v>57</v>
       </c>
-      <c r="E12" t="s" s="486">
-        <v>84</v>
-      </c>
-      <c r="F12" t="s" s="487">
-        <v>60</v>
-      </c>
-      <c r="G12" t="s" s="488">
-        <v>61</v>
-      </c>
-      <c r="H12" t="s" s="489">
+      <c r="Q12" t="s">
         <v>58</v>
-      </c>
-      <c r="I12" t="s" s="490">
-        <v>85</v>
-      </c>
-      <c r="J12" t="s" s="491">
-        <v>84</v>
-      </c>
-      <c r="K12" t="s" s="492">
-        <v>57</v>
-      </c>
-      <c r="L12" t="s" s="493">
-        <v>57</v>
-      </c>
-      <c r="M12" t="s" s="494">
-        <v>85</v>
-      </c>
-      <c r="N12" t="s" s="495">
-        <v>56</v>
-      </c>
-      <c r="O12" t="s" s="496">
-        <v>63</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s" s="497">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B13" t="n" s="498">
         <v>14.0</v>
       </c>
       <c r="C13" s="499"/>
       <c r="D13" t="s" s="500">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E13" t="s" s="501">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="F13" t="s" s="502">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="G13" t="s" s="503">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="H13" t="s" s="504">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="I13" t="s" s="505">
+        <v>50</v>
+      </c>
+      <c r="J13" t="s" s="506">
+        <v>116</v>
+      </c>
+      <c r="K13" t="s" s="507">
+        <v>177</v>
+      </c>
+      <c r="L13" t="s" s="508">
+        <v>50</v>
+      </c>
+      <c r="M13" t="s" s="509">
+        <v>134</v>
+      </c>
+      <c r="N13" t="s" s="510">
+        <v>48</v>
+      </c>
+      <c r="O13" t="s" s="511">
+        <v>55</v>
+      </c>
+      <c r="P13" t="s">
+        <v>57</v>
+      </c>
+      <c r="Q13" t="s">
         <v>58</v>
-      </c>
-      <c r="J13" t="s" s="506">
-        <v>119</v>
-      </c>
-      <c r="K13" t="s" s="507">
-        <v>174</v>
-      </c>
-      <c r="L13" t="s" s="508">
-        <v>58</v>
-      </c>
-      <c r="M13" t="s" s="509">
-        <v>136</v>
-      </c>
-      <c r="N13" t="s" s="510">
-        <v>56</v>
-      </c>
-      <c r="O13" t="s" s="511">
-        <v>63</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s" s="512">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="B14" t="n" s="513">
         <v>14.0</v>
       </c>
       <c r="C14" s="514"/>
       <c r="D14" t="s" s="515">
+        <v>49</v>
+      </c>
+      <c r="E14" t="s" s="516">
+        <v>47</v>
+      </c>
+      <c r="F14" t="s" s="517">
+        <v>52</v>
+      </c>
+      <c r="G14" t="s" s="518">
+        <v>83</v>
+      </c>
+      <c r="H14" t="s" s="519">
+        <v>56</v>
+      </c>
+      <c r="I14" t="s" s="520">
+        <v>54</v>
+      </c>
+      <c r="J14" t="s" s="521">
+        <v>79</v>
+      </c>
+      <c r="K14" t="s" s="522">
+        <v>56</v>
+      </c>
+      <c r="L14" t="s" s="523">
+        <v>56</v>
+      </c>
+      <c r="M14" t="s" s="524">
+        <v>80</v>
+      </c>
+      <c r="N14" t="s" s="525">
+        <v>48</v>
+      </c>
+      <c r="O14" t="s" s="526">
+        <v>55</v>
+      </c>
+      <c r="P14" t="s">
         <v>57</v>
       </c>
-      <c r="E14" t="s" s="516">
-        <v>55</v>
-      </c>
-      <c r="F14" t="s" s="517">
-        <v>60</v>
-      </c>
-      <c r="G14" t="s" s="518">
-        <v>88</v>
-      </c>
-      <c r="H14" t="s" s="519">
-        <v>64</v>
-      </c>
-      <c r="I14" t="s" s="520">
-        <v>62</v>
-      </c>
-      <c r="J14" t="s" s="521">
-        <v>84</v>
-      </c>
-      <c r="K14" t="s" s="522">
-        <v>64</v>
-      </c>
-      <c r="L14" t="s" s="523">
-        <v>64</v>
-      </c>
-      <c r="M14" t="s" s="524">
-        <v>85</v>
-      </c>
-      <c r="N14" t="s" s="525">
-        <v>56</v>
-      </c>
-      <c r="O14" t="s" s="526">
-        <v>63</v>
+      <c r="Q14" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s" s="527">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B15" t="n" s="528">
         <v>14.0</v>
       </c>
       <c r="C15" s="529"/>
       <c r="D15" t="s" s="530">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E15" t="s" s="531">
+        <v>47</v>
+      </c>
+      <c r="F15" t="s" s="532">
+        <v>52</v>
+      </c>
+      <c r="G15" t="s" s="533">
+        <v>83</v>
+      </c>
+      <c r="H15" t="s" s="534">
+        <v>49</v>
+      </c>
+      <c r="I15" t="s" s="535">
+        <v>50</v>
+      </c>
+      <c r="J15" t="s" s="536">
+        <v>79</v>
+      </c>
+      <c r="K15" t="s" s="537">
+        <v>49</v>
+      </c>
+      <c r="L15" t="s" s="538">
+        <v>177</v>
+      </c>
+      <c r="M15" t="s" s="539">
+        <v>177</v>
+      </c>
+      <c r="N15" t="s" s="540">
+        <v>48</v>
+      </c>
+      <c r="O15" t="s" s="541">
         <v>55</v>
       </c>
-      <c r="F15" t="s" s="532">
-        <v>60</v>
-      </c>
-      <c r="G15" t="s" s="533">
-        <v>88</v>
-      </c>
-      <c r="H15" t="s" s="534">
+      <c r="P15" t="s">
         <v>57</v>
       </c>
-      <c r="I15" t="s" s="535">
+      <c r="Q15" t="s">
         <v>58</v>
-      </c>
-      <c r="J15" t="s" s="536">
-        <v>84</v>
-      </c>
-      <c r="K15" t="s" s="537">
-        <v>57</v>
-      </c>
-      <c r="L15" t="s" s="538">
-        <v>174</v>
-      </c>
-      <c r="M15" t="s" s="539">
-        <v>174</v>
-      </c>
-      <c r="N15" t="s" s="540">
-        <v>56</v>
-      </c>
-      <c r="O15" t="s" s="541">
-        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -6956,7 +7530,7 @@
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="N2:O2"/>
-    <mergeCell ref="P1:AA1"/>
+    <mergeCell ref="P1:R1"/>
     <mergeCell ref="P2:U2"/>
     <mergeCell ref="V2:Z2"/>
   </mergeCells>

</xml_diff>